<commit_message>
Export Driver Report to html and xlsx
</commit_message>
<xml_diff>
--- a/Service/src/main/resources/templates/regionReport.xlsx
+++ b/Service/src/main/resources/templates/regionReport.xlsx
@@ -324,7 +324,7 @@
       <c r="C4" s="3" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-26T17:49:45.727032200</t>
+            <t xml:space="preserve">2023-11-26T19:35:16</t>
           </r>
         </is>
       </c>
@@ -827,18 +827,18 @@
     </row>
     <row r="19" customHeight="1" ht="1">
       <c r="A19" s="1" t="inlineStr"/>
-      <c r="B19" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-10-29T15:46:57</t>
-          </r>
-        </is>
-      </c>
-      <c r="C19" s="6" t="inlineStr"/>
+      <c r="B19" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-10-29T16:04</t>
+          </r>
+        </is>
+      </c>
+      <c r="C19" s="8" t="inlineStr"/>
       <c r="D19" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">er</t>
+            <t xml:space="preserve">nop</t>
           </r>
         </is>
       </c>
@@ -853,7 +853,7 @@
       <c r="G19" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -877,7 +877,7 @@
       <c r="M19" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">another</t>
           </r>
         </is>
       </c>
@@ -890,8 +890,8 @@
     </row>
     <row r="20" customHeight="1" ht="29">
       <c r="A20" s="1" t="inlineStr"/>
-      <c r="B20" s="6" t="inlineStr"/>
-      <c r="C20" s="6" t="inlineStr"/>
+      <c r="B20" s="8" t="inlineStr"/>
+      <c r="C20" s="8" t="inlineStr"/>
       <c r="D20" s="7" t="inlineStr"/>
       <c r="E20" s="7" t="inlineStr"/>
       <c r="F20" s="7" t="inlineStr"/>
@@ -906,21 +906,21 @@
       <c r="O20" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">21</t>
           </r>
         </is>
       </c>
       <c r="P20" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">321654</t>
           </r>
         </is>
       </c>
       <c r="Q20" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">7</t>
+            <t xml:space="preserve">12</t>
           </r>
         </is>
       </c>
@@ -974,7 +974,7 @@
       <c r="B23" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T15:48:12</t>
+            <t xml:space="preserve">2023-10-29T16:29:39</t>
           </r>
         </is>
       </c>
@@ -982,7 +982,7 @@
       <c r="D23" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">er</t>
+            <t xml:space="preserve">notes</t>
           </r>
         </is>
       </c>
@@ -997,7 +997,7 @@
       <c r="G23" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="M23" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">another</t>
           </r>
         </is>
       </c>
@@ -1050,21 +1050,21 @@
       <c r="O24" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">22</t>
           </r>
         </is>
       </c>
       <c r="P24" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">321654</t>
           </r>
         </is>
       </c>
       <c r="Q24" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">8</t>
+            <t xml:space="preserve">13</t>
           </r>
         </is>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="B27" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T15:50:38</t>
+            <t xml:space="preserve">2023-10-29T16:59:46</t>
           </r>
         </is>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="D27" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">er</t>
+            <t xml:space="preserve">notest</t>
           </r>
         </is>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="G27" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -1165,7 +1165,7 @@
       <c r="M27" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">another</t>
           </r>
         </is>
       </c>
@@ -1194,21 +1194,21 @@
       <c r="O28" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">23</t>
           </r>
         </is>
       </c>
       <c r="P28" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">321654</t>
           </r>
         </is>
       </c>
       <c r="Q28" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">9</t>
+            <t xml:space="preserve">14</t>
           </r>
         </is>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="B31" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T15:51:28</t>
+            <t xml:space="preserve">2023-10-29T21:37:51</t>
           </r>
         </is>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="D31" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">er</t>
+            <t xml:space="preserve">yu</t>
           </r>
         </is>
       </c>
@@ -1285,7 +1285,7 @@
       <c r="G31" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="M31" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">another</t>
           </r>
         </is>
       </c>
@@ -1338,21 +1338,21 @@
       <c r="O32" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">25</t>
           </r>
         </is>
       </c>
       <c r="P32" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">321654</t>
           </r>
         </is>
       </c>
       <c r="Q32" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">10</t>
+            <t xml:space="preserve">17</t>
           </r>
         </is>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="B35" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T15:57:11</t>
+            <t xml:space="preserve">2023-10-29T22:00:42</t>
           </r>
         </is>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="D35" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">er</t>
+            <t xml:space="preserve">uo</t>
           </r>
         </is>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="G35" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="M35" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">another</t>
           </r>
         </is>
       </c>
@@ -1482,21 +1482,21 @@
       <c r="O36" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">26</t>
           </r>
         </is>
       </c>
       <c r="P36" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">null</t>
+            <t xml:space="preserve">321654</t>
           </r>
         </is>
       </c>
       <c r="Q36" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">11</t>
+            <t xml:space="preserve">18</t>
           </r>
         </is>
       </c>
@@ -1547,18 +1547,18 @@
     </row>
     <row r="39" customHeight="1" ht="1">
       <c r="A39" s="1" t="inlineStr"/>
-      <c r="B39" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-10-29T16:04</t>
-          </r>
-        </is>
-      </c>
-      <c r="C39" s="8" t="inlineStr"/>
+      <c r="B39" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-10-29T22:01:28</t>
+          </r>
+        </is>
+      </c>
+      <c r="C39" s="6" t="inlineStr"/>
       <c r="D39" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">nop</t>
+            <t xml:space="preserve">3</t>
           </r>
         </is>
       </c>
@@ -1610,8 +1610,8 @@
     </row>
     <row r="40" customHeight="1" ht="29">
       <c r="A40" s="1" t="inlineStr"/>
-      <c r="B40" s="8" t="inlineStr"/>
-      <c r="C40" s="8" t="inlineStr"/>
+      <c r="B40" s="6" t="inlineStr"/>
+      <c r="C40" s="6" t="inlineStr"/>
       <c r="D40" s="7" t="inlineStr"/>
       <c r="E40" s="7" t="inlineStr"/>
       <c r="F40" s="7" t="inlineStr"/>
@@ -1626,7 +1626,7 @@
       <c r="O40" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">21</t>
+            <t xml:space="preserve">27</t>
           </r>
         </is>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="Q40" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">12</t>
+            <t xml:space="preserve">19</t>
           </r>
         </is>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="B43" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T16:29:39</t>
+            <t xml:space="preserve">2023-10-29T22:02:43</t>
           </r>
         </is>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="D43" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">notes</t>
+            <t xml:space="preserve">344</t>
           </r>
         </is>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="G43" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref1</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -1770,7 +1770,7 @@
       <c r="O44" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">22</t>
+            <t xml:space="preserve">28</t>
           </r>
         </is>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="Q44" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">13</t>
+            <t xml:space="preserve">20</t>
           </r>
         </is>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="B47" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T16:59:46</t>
+            <t xml:space="preserve">2023-10-29T22:07:36</t>
           </r>
         </is>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="D47" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">notest</t>
+            <t xml:space="preserve">344</t>
           </r>
         </is>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="G47" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref1</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="O48" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">23</t>
+            <t xml:space="preserve">28</t>
           </r>
         </is>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="Q48" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">14</t>
+            <t xml:space="preserve">21</t>
           </r>
         </is>
       </c>
@@ -1982,7 +1982,7 @@
       <c r="B51" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T21:37:51</t>
+            <t xml:space="preserve">2023-10-29T22:10:57</t>
           </r>
         </is>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="D51" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">yu</t>
+            <t xml:space="preserve">w</t>
           </r>
         </is>
       </c>
@@ -2005,7 +2005,7 @@
       <c r="G51" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="O52" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">25</t>
+            <t xml:space="preserve">29</t>
           </r>
         </is>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="Q52" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">17</t>
+            <t xml:space="preserve">22</t>
           </r>
         </is>
       </c>
@@ -2126,7 +2126,7 @@
       <c r="B55" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:00:42</t>
+            <t xml:space="preserve">2023-10-29T22:13:47</t>
           </r>
         </is>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="D55" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">uo</t>
+            <t xml:space="preserve">344</t>
           </r>
         </is>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="G55" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="O56" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">26</t>
+            <t xml:space="preserve">30</t>
           </r>
         </is>
       </c>
@@ -2216,7 +2216,7 @@
       <c r="Q56" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">18</t>
+            <t xml:space="preserve">23</t>
           </r>
         </is>
       </c>
@@ -2270,7 +2270,7 @@
       <c r="B59" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:01:28</t>
+            <t xml:space="preserve">2023-10-29T22:15:50</t>
           </r>
         </is>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="D59" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">344</t>
           </r>
         </is>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="O60" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">27</t>
+            <t xml:space="preserve">30</t>
           </r>
         </is>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="Q60" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">19</t>
+            <t xml:space="preserve">24</t>
           </r>
         </is>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="B63" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:02:43</t>
+            <t xml:space="preserve">2023-10-29T22:19:14</t>
           </r>
         </is>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="D63" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">344</t>
+            <t xml:space="preserve">pp</t>
           </r>
         </is>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="O64" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">28</t>
+            <t xml:space="preserve">31</t>
           </r>
         </is>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="Q64" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">20</t>
+            <t xml:space="preserve">25</t>
           </r>
         </is>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="B67" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:07:36</t>
+            <t xml:space="preserve">2023-10-29T22:20:44</t>
           </r>
         </is>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="D67" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">344</t>
+            <t xml:space="preserve">re</t>
           </r>
         </is>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="G67" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -2634,7 +2634,7 @@
       <c r="O68" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">28</t>
+            <t xml:space="preserve">32</t>
           </r>
         </is>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="Q68" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">21</t>
+            <t xml:space="preserve">27</t>
           </r>
         </is>
       </c>
@@ -2702,7 +2702,7 @@
       <c r="B71" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:10:57</t>
+            <t xml:space="preserve">2023-10-29T22:27:07</t>
           </r>
         </is>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="D71" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">w</t>
+            <t xml:space="preserve">23</t>
           </r>
         </is>
       </c>
@@ -2741,7 +2741,7 @@
       <c r="K71" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">20000</t>
           </r>
         </is>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="O72" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">29</t>
+            <t xml:space="preserve">33</t>
           </r>
         </is>
       </c>
@@ -2792,7 +2792,7 @@
       <c r="Q72" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">22</t>
+            <t xml:space="preserve">30</t>
           </r>
         </is>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="B75" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:13:47</t>
+            <t xml:space="preserve">2023-11-01T21:25:46</t>
           </r>
         </is>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="D75" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">344</t>
+            <t xml:space="preserve">78</t>
           </r>
         </is>
       </c>
@@ -2869,7 +2869,7 @@
       <c r="G75" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref1</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -2885,7 +2885,7 @@
       <c r="K75" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">40000</t>
           </r>
         </is>
       </c>
@@ -2922,7 +2922,7 @@
       <c r="O76" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">30</t>
+            <t xml:space="preserve">35</t>
           </r>
         </is>
       </c>
@@ -2936,7 +2936,7 @@
       <c r="Q76" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">23</t>
+            <t xml:space="preserve">34</t>
           </r>
         </is>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="B79" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:15:50</t>
+            <t xml:space="preserve">2023-11-01T21:28:26</t>
           </r>
         </is>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="D79" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">344</t>
+            <t xml:space="preserve">notes</t>
           </r>
         </is>
       </c>
@@ -3029,7 +3029,7 @@
       <c r="K79" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">40000</t>
           </r>
         </is>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="O80" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">30</t>
+            <t xml:space="preserve">36</t>
           </r>
         </is>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="Q80" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">24</t>
+            <t xml:space="preserve">36</t>
           </r>
         </is>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="B88" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:19:14</t>
+            <t xml:space="preserve">2023-11-01T21:30:22</t>
           </r>
         </is>
       </c>
@@ -3313,7 +3313,7 @@
       <c r="D88" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">pp</t>
+            <t xml:space="preserve">test</t>
           </r>
         </is>
       </c>
@@ -3328,7 +3328,7 @@
       <c r="G88" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -3344,7 +3344,7 @@
       <c r="K88" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">25000</t>
           </r>
         </is>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="O89" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">31</t>
+            <t xml:space="preserve">37</t>
           </r>
         </is>
       </c>
@@ -3395,7 +3395,7 @@
       <c r="Q89" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">25</t>
+            <t xml:space="preserve">37</t>
           </r>
         </is>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="B92" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:20:44</t>
+            <t xml:space="preserve">2023-11-01T21:32:09</t>
           </r>
         </is>
       </c>
@@ -3457,7 +3457,7 @@
       <c r="D92" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">re</t>
+            <t xml:space="preserve">test note</t>
           </r>
         </is>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="G92" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref1</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -3488,7 +3488,7 @@
       <c r="K92" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">25000</t>
           </r>
         </is>
       </c>
@@ -3525,7 +3525,7 @@
       <c r="O93" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">32</t>
+            <t xml:space="preserve">38</t>
           </r>
         </is>
       </c>
@@ -3539,7 +3539,7 @@
       <c r="Q93" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">27</t>
+            <t xml:space="preserve">39</t>
           </r>
         </is>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="B96" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-10-29T22:27:07</t>
+            <t xml:space="preserve">2023-11-01T21:32:25</t>
           </r>
         </is>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="D96" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">23</t>
+            <t xml:space="preserve">test note</t>
           </r>
         </is>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="G96" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref1</t>
+            <t xml:space="preserve">ref2</t>
           </r>
         </is>
       </c>
@@ -3625,7 +3625,7 @@
       <c r="J96" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">mat2</t>
+            <t xml:space="preserve">mat1</t>
           </r>
         </is>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="O97" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">33</t>
+            <t xml:space="preserve">38</t>
           </r>
         </is>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="Q97" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">30</t>
+            <t xml:space="preserve">40</t>
           </r>
         </is>
       </c>
@@ -3737,7 +3737,7 @@
       <c r="B100" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T21:25:46</t>
+            <t xml:space="preserve">2023-11-01T21:48:06</t>
           </r>
         </is>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="D100" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">78</t>
+            <t xml:space="preserve">notes</t>
           </r>
         </is>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="G100" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -3776,7 +3776,7 @@
       <c r="K100" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">40000</t>
+            <t xml:space="preserve">45000</t>
           </r>
         </is>
       </c>
@@ -3813,7 +3813,7 @@
       <c r="O101" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">35</t>
+            <t xml:space="preserve">39</t>
           </r>
         </is>
       </c>
@@ -3827,7 +3827,7 @@
       <c r="Q101" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">34</t>
+            <t xml:space="preserve">41</t>
           </r>
         </is>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="B104" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T21:28:26</t>
+            <t xml:space="preserve">2023-11-01T22:11:38</t>
           </r>
         </is>
       </c>
@@ -3889,7 +3889,7 @@
       <c r="D104" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">notes</t>
+            <t xml:space="preserve">re</t>
           </r>
         </is>
       </c>
@@ -3920,7 +3920,7 @@
       <c r="K104" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">40000</t>
+            <t xml:space="preserve">45000</t>
           </r>
         </is>
       </c>
@@ -3957,7 +3957,7 @@
       <c r="O105" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">36</t>
+            <t xml:space="preserve">40</t>
           </r>
         </is>
       </c>
@@ -3971,7 +3971,7 @@
       <c r="Q105" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">36</t>
+            <t xml:space="preserve">42</t>
           </r>
         </is>
       </c>
@@ -4025,7 +4025,7 @@
       <c r="B108" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T21:30:22</t>
+            <t xml:space="preserve">2023-11-01T22:13:30</t>
           </r>
         </is>
       </c>
@@ -4033,7 +4033,7 @@
       <c r="D108" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">test</t>
+            <t xml:space="preserve">note</t>
           </r>
         </is>
       </c>
@@ -4064,7 +4064,7 @@
       <c r="K108" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">25000</t>
+            <t xml:space="preserve">45000</t>
           </r>
         </is>
       </c>
@@ -4101,7 +4101,7 @@
       <c r="O109" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">37</t>
+            <t xml:space="preserve">41</t>
           </r>
         </is>
       </c>
@@ -4115,7 +4115,7 @@
       <c r="Q109" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">37</t>
+            <t xml:space="preserve">43</t>
           </r>
         </is>
       </c>
@@ -4169,7 +4169,7 @@
       <c r="B112" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T21:32:09</t>
+            <t xml:space="preserve">2023-11-01T22:15:31</t>
           </r>
         </is>
       </c>
@@ -4177,7 +4177,7 @@
       <c r="D112" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">test note</t>
+            <t xml:space="preserve">mm</t>
           </r>
         </is>
       </c>
@@ -4192,7 +4192,7 @@
       <c r="G112" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="K112" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">25000</t>
+            <t xml:space="preserve">45000</t>
           </r>
         </is>
       </c>
@@ -4245,7 +4245,7 @@
       <c r="O113" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">38</t>
+            <t xml:space="preserve">42</t>
           </r>
         </is>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="Q113" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">39</t>
+            <t xml:space="preserve">44</t>
           </r>
         </is>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="B116" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T21:32:25</t>
+            <t xml:space="preserve">2023-11-01T22:27:47</t>
           </r>
         </is>
       </c>
@@ -4321,7 +4321,7 @@
       <c r="D116" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">test note</t>
+            <t xml:space="preserve">w</t>
           </r>
         </is>
       </c>
@@ -4336,7 +4336,7 @@
       <c r="G116" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">ref2</t>
+            <t xml:space="preserve">ref1</t>
           </r>
         </is>
       </c>
@@ -4345,14 +4345,14 @@
       <c r="J116" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">mat1</t>
+            <t xml:space="preserve">mat2</t>
           </r>
         </is>
       </c>
       <c r="K116" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">20000</t>
+            <t xml:space="preserve">45000</t>
           </r>
         </is>
       </c>
@@ -4389,7 +4389,7 @@
       <c r="O117" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">38</t>
+            <t xml:space="preserve">43</t>
           </r>
         </is>
       </c>
@@ -4403,7 +4403,7 @@
       <c r="Q117" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">40</t>
+            <t xml:space="preserve">45</t>
           </r>
         </is>
       </c>
@@ -4457,7 +4457,7 @@
       <c r="B120" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T21:48:06</t>
+            <t xml:space="preserve">2023-11-04T21:11:17</t>
           </r>
         </is>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="D120" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">notes</t>
+            <t xml:space="preserve">your notes</t>
           </r>
         </is>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="K120" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">36000</t>
           </r>
         </is>
       </c>
@@ -4504,7 +4504,7 @@
       <c r="M120" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">another</t>
+            <t xml:space="preserve">pers</t>
           </r>
         </is>
       </c>
@@ -4533,21 +4533,21 @@
       <c r="O121" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">39</t>
+            <t xml:space="preserve">44</t>
           </r>
         </is>
       </c>
       <c r="P121" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">321654</t>
+            <t xml:space="preserve">980980</t>
           </r>
         </is>
       </c>
       <c r="Q121" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">41</t>
+            <t xml:space="preserve">46</t>
           </r>
         </is>
       </c>
@@ -4601,7 +4601,7 @@
       <c r="B124" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T22:11:38</t>
+            <t xml:space="preserve">2023-11-04T21:13:31</t>
           </r>
         </is>
       </c>
@@ -4609,7 +4609,7 @@
       <c r="D124" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">re</t>
+            <t xml:space="preserve">eee</t>
           </r>
         </is>
       </c>
@@ -4640,7 +4640,7 @@
       <c r="K124" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">36000</t>
           </r>
         </is>
       </c>
@@ -4648,7 +4648,7 @@
       <c r="M124" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">another</t>
+            <t xml:space="preserve">pers</t>
           </r>
         </is>
       </c>
@@ -4677,21 +4677,21 @@
       <c r="O125" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">40</t>
+            <t xml:space="preserve">45</t>
           </r>
         </is>
       </c>
       <c r="P125" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">321654</t>
+            <t xml:space="preserve">980980</t>
           </r>
         </is>
       </c>
       <c r="Q125" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">42</t>
+            <t xml:space="preserve">47</t>
           </r>
         </is>
       </c>
@@ -4745,7 +4745,7 @@
       <c r="B128" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T22:13:30</t>
+            <t xml:space="preserve">2023-11-04T22:03:37</t>
           </r>
         </is>
       </c>
@@ -4753,7 +4753,7 @@
       <c r="D128" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">note</t>
+            <t xml:space="preserve">3ew</t>
           </r>
         </is>
       </c>
@@ -4784,7 +4784,7 @@
       <c r="K128" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">36000</t>
           </r>
         </is>
       </c>
@@ -4792,7 +4792,7 @@
       <c r="M128" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">another</t>
+            <t xml:space="preserve">pers</t>
           </r>
         </is>
       </c>
@@ -4821,21 +4821,21 @@
       <c r="O129" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">41</t>
+            <t xml:space="preserve">48</t>
           </r>
         </is>
       </c>
       <c r="P129" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">321654</t>
+            <t xml:space="preserve">980980</t>
           </r>
         </is>
       </c>
       <c r="Q129" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">43</t>
+            <t xml:space="preserve">48</t>
           </r>
         </is>
       </c>
@@ -4889,7 +4889,7 @@
       <c r="B132" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T22:15:31</t>
+            <t xml:space="preserve">2023-11-04T22:31:40</t>
           </r>
         </is>
       </c>
@@ -4897,7 +4897,7 @@
       <c r="D132" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">mm</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -4928,7 +4928,7 @@
       <c r="K132" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45000</t>
+            <t xml:space="preserve">36000</t>
           </r>
         </is>
       </c>
@@ -4936,7 +4936,7 @@
       <c r="M132" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">another</t>
+            <t xml:space="preserve">pers</t>
           </r>
         </is>
       </c>
@@ -4965,21 +4965,21 @@
       <c r="O133" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">42</t>
+            <t xml:space="preserve">49</t>
           </r>
         </is>
       </c>
       <c r="P133" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">321654</t>
+            <t xml:space="preserve">980980</t>
           </r>
         </is>
       </c>
       <c r="Q133" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">44</t>
+            <t xml:space="preserve">49</t>
           </r>
         </is>
       </c>
@@ -5033,7 +5033,7 @@
       <c r="B136" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-01T22:27:47</t>
+            <t xml:space="preserve">2023-11-04T22:40:28</t>
           </r>
         </is>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="O137" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">43</t>
+            <t xml:space="preserve">50</t>
           </r>
         </is>
       </c>
@@ -5123,7 +5123,7 @@
       <c r="Q137" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45</t>
+            <t xml:space="preserve">50</t>
           </r>
         </is>
       </c>
@@ -5177,7 +5177,7 @@
       <c r="B140" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-04T21:11:17</t>
+            <t xml:space="preserve">2023-11-05T00:02:45</t>
           </r>
         </is>
       </c>
@@ -5185,7 +5185,7 @@
       <c r="D140" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">your notes</t>
+            <t xml:space="preserve">notes</t>
           </r>
         </is>
       </c>
@@ -5253,7 +5253,7 @@
       <c r="O141" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">44</t>
+            <t xml:space="preserve">51</t>
           </r>
         </is>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="Q141" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">46</t>
+            <t xml:space="preserve">51</t>
           </r>
         </is>
       </c>
@@ -5321,7 +5321,7 @@
       <c r="B144" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-04T21:13:31</t>
+            <t xml:space="preserve">2023-11-05T00:31:39</t>
           </r>
         </is>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="D144" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">eee</t>
+            <t xml:space="preserve">b</t>
           </r>
         </is>
       </c>
@@ -5397,7 +5397,7 @@
       <c r="O145" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">45</t>
+            <t xml:space="preserve">52</t>
           </r>
         </is>
       </c>
@@ -5411,7 +5411,7 @@
       <c r="Q145" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">47</t>
+            <t xml:space="preserve">52</t>
           </r>
         </is>
       </c>
@@ -5465,7 +5465,7 @@
       <c r="B148" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-04T22:03:37</t>
+            <t xml:space="preserve">2023-11-05T00:35:07</t>
           </r>
         </is>
       </c>
@@ -5473,7 +5473,7 @@
       <c r="D148" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">3ew</t>
+            <t xml:space="preserve">90</t>
           </r>
         </is>
       </c>
@@ -5541,7 +5541,7 @@
       <c r="O149" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">48</t>
+            <t xml:space="preserve">53</t>
           </r>
         </is>
       </c>
@@ -5555,7 +5555,7 @@
       <c r="Q149" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">48</t>
+            <t xml:space="preserve">53</t>
           </r>
         </is>
       </c>
@@ -5609,7 +5609,7 @@
       <c r="B152" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-04T22:31:40</t>
+            <t xml:space="preserve">2023-11-05T20:56:37</t>
           </r>
         </is>
       </c>
@@ -5617,7 +5617,7 @@
       <c r="D152" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">cftyfyt</t>
           </r>
         </is>
       </c>
@@ -5648,7 +5648,7 @@
       <c r="K152" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">36000</t>
+            <t xml:space="preserve">45000</t>
           </r>
         </is>
       </c>
@@ -5656,7 +5656,7 @@
       <c r="M152" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">pers</t>
+            <t xml:space="preserve">another</t>
           </r>
         </is>
       </c>
@@ -5685,21 +5685,21 @@
       <c r="O153" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">49</t>
+            <t xml:space="preserve">54</t>
           </r>
         </is>
       </c>
       <c r="P153" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">980980</t>
+            <t xml:space="preserve">321654</t>
           </r>
         </is>
       </c>
       <c r="Q153" s="7" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">49</t>
+            <t xml:space="preserve">54</t>
           </r>
         </is>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="R154" s="1" t="inlineStr"/>
       <c r="S154" s="1" t="inlineStr"/>
     </row>
-    <row r="155" customHeight="1" ht="5">
+    <row r="155" customHeight="1" ht="160">
       <c r="A155" s="1" t="inlineStr"/>
       <c r="B155" s="1" t="inlineStr"/>
       <c r="C155" s="1" t="inlineStr"/>
@@ -5747,2193 +5747,6 @@
       <c r="Q155" s="1" t="inlineStr"/>
       <c r="R155" s="1" t="inlineStr"/>
       <c r="S155" s="1" t="inlineStr"/>
-    </row>
-    <row r="156" customHeight="1" ht="1">
-      <c r="A156" s="1" t="inlineStr"/>
-      <c r="B156" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-04T22:40:28</t>
-          </r>
-        </is>
-      </c>
-      <c r="C156" s="6" t="inlineStr"/>
-      <c r="D156" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">w</t>
-          </r>
-        </is>
-      </c>
-      <c r="E156" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F156" s="7" t="inlineStr"/>
-      <c r="G156" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H156" s="7" t="inlineStr"/>
-      <c r="I156" s="7" t="inlineStr"/>
-      <c r="J156" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K156" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">45000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L156" s="7" t="inlineStr"/>
-      <c r="M156" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">another</t>
-          </r>
-        </is>
-      </c>
-      <c r="N156" s="7" t="inlineStr"/>
-      <c r="O156" s="1" t="inlineStr"/>
-      <c r="P156" s="1" t="inlineStr"/>
-      <c r="Q156" s="1" t="inlineStr"/>
-      <c r="R156" s="1" t="inlineStr"/>
-      <c r="S156" s="1" t="inlineStr"/>
-    </row>
-    <row r="157" customHeight="1" ht="29">
-      <c r="A157" s="1" t="inlineStr"/>
-      <c r="B157" s="6" t="inlineStr"/>
-      <c r="C157" s="6" t="inlineStr"/>
-      <c r="D157" s="7" t="inlineStr"/>
-      <c r="E157" s="7" t="inlineStr"/>
-      <c r="F157" s="7" t="inlineStr"/>
-      <c r="G157" s="7" t="inlineStr"/>
-      <c r="H157" s="7" t="inlineStr"/>
-      <c r="I157" s="7" t="inlineStr"/>
-      <c r="J157" s="7" t="inlineStr"/>
-      <c r="K157" s="7" t="inlineStr"/>
-      <c r="L157" s="7" t="inlineStr"/>
-      <c r="M157" s="7" t="inlineStr"/>
-      <c r="N157" s="7" t="inlineStr"/>
-      <c r="O157" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">50</t>
-          </r>
-        </is>
-      </c>
-      <c r="P157" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">321654</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q157" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">50</t>
-          </r>
-        </is>
-      </c>
-      <c r="R157" s="1" t="inlineStr"/>
-      <c r="S157" s="1" t="inlineStr"/>
-    </row>
-    <row r="158" customHeight="1" ht="1">
-      <c r="A158" s="1" t="inlineStr"/>
-      <c r="B158" s="1" t="inlineStr"/>
-      <c r="C158" s="1" t="inlineStr"/>
-      <c r="D158" s="1" t="inlineStr"/>
-      <c r="E158" s="1" t="inlineStr"/>
-      <c r="F158" s="1" t="inlineStr"/>
-      <c r="G158" s="1" t="inlineStr"/>
-      <c r="H158" s="1" t="inlineStr"/>
-      <c r="I158" s="1" t="inlineStr"/>
-      <c r="J158" s="1" t="inlineStr"/>
-      <c r="K158" s="1" t="inlineStr"/>
-      <c r="L158" s="1" t="inlineStr"/>
-      <c r="M158" s="1" t="inlineStr"/>
-      <c r="N158" s="1" t="inlineStr"/>
-      <c r="O158" s="7" t="inlineStr"/>
-      <c r="P158" s="7" t="inlineStr"/>
-      <c r="Q158" s="7" t="inlineStr"/>
-      <c r="R158" s="1" t="inlineStr"/>
-      <c r="S158" s="1" t="inlineStr"/>
-    </row>
-    <row r="159" customHeight="1" ht="5">
-      <c r="A159" s="1" t="inlineStr"/>
-      <c r="B159" s="1" t="inlineStr"/>
-      <c r="C159" s="1" t="inlineStr"/>
-      <c r="D159" s="1" t="inlineStr"/>
-      <c r="E159" s="1" t="inlineStr"/>
-      <c r="F159" s="1" t="inlineStr"/>
-      <c r="G159" s="1" t="inlineStr"/>
-      <c r="H159" s="1" t="inlineStr"/>
-      <c r="I159" s="1" t="inlineStr"/>
-      <c r="J159" s="1" t="inlineStr"/>
-      <c r="K159" s="1" t="inlineStr"/>
-      <c r="L159" s="1" t="inlineStr"/>
-      <c r="M159" s="1" t="inlineStr"/>
-      <c r="N159" s="1" t="inlineStr"/>
-      <c r="O159" s="1" t="inlineStr"/>
-      <c r="P159" s="1" t="inlineStr"/>
-      <c r="Q159" s="1" t="inlineStr"/>
-      <c r="R159" s="1" t="inlineStr"/>
-      <c r="S159" s="1" t="inlineStr"/>
-    </row>
-    <row r="160" customHeight="1" ht="1">
-      <c r="A160" s="1" t="inlineStr"/>
-      <c r="B160" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-05T00:02:45</t>
-          </r>
-        </is>
-      </c>
-      <c r="C160" s="6" t="inlineStr"/>
-      <c r="D160" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">notes</t>
-          </r>
-        </is>
-      </c>
-      <c r="E160" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F160" s="7" t="inlineStr"/>
-      <c r="G160" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H160" s="7" t="inlineStr"/>
-      <c r="I160" s="7" t="inlineStr"/>
-      <c r="J160" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K160" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">36000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L160" s="7" t="inlineStr"/>
-      <c r="M160" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N160" s="7" t="inlineStr"/>
-      <c r="O160" s="1" t="inlineStr"/>
-      <c r="P160" s="1" t="inlineStr"/>
-      <c r="Q160" s="1" t="inlineStr"/>
-      <c r="R160" s="1" t="inlineStr"/>
-      <c r="S160" s="1" t="inlineStr"/>
-    </row>
-    <row r="161" customHeight="1" ht="29">
-      <c r="A161" s="1" t="inlineStr"/>
-      <c r="B161" s="6" t="inlineStr"/>
-      <c r="C161" s="6" t="inlineStr"/>
-      <c r="D161" s="7" t="inlineStr"/>
-      <c r="E161" s="7" t="inlineStr"/>
-      <c r="F161" s="7" t="inlineStr"/>
-      <c r="G161" s="7" t="inlineStr"/>
-      <c r="H161" s="7" t="inlineStr"/>
-      <c r="I161" s="7" t="inlineStr"/>
-      <c r="J161" s="7" t="inlineStr"/>
-      <c r="K161" s="7" t="inlineStr"/>
-      <c r="L161" s="7" t="inlineStr"/>
-      <c r="M161" s="7" t="inlineStr"/>
-      <c r="N161" s="7" t="inlineStr"/>
-      <c r="O161" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">51</t>
-          </r>
-        </is>
-      </c>
-      <c r="P161" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q161" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">51</t>
-          </r>
-        </is>
-      </c>
-      <c r="R161" s="1" t="inlineStr"/>
-      <c r="S161" s="1" t="inlineStr"/>
-    </row>
-    <row r="162" customHeight="1" ht="1">
-      <c r="A162" s="1" t="inlineStr"/>
-      <c r="B162" s="1" t="inlineStr"/>
-      <c r="C162" s="1" t="inlineStr"/>
-      <c r="D162" s="1" t="inlineStr"/>
-      <c r="E162" s="1" t="inlineStr"/>
-      <c r="F162" s="1" t="inlineStr"/>
-      <c r="G162" s="1" t="inlineStr"/>
-      <c r="H162" s="1" t="inlineStr"/>
-      <c r="I162" s="1" t="inlineStr"/>
-      <c r="J162" s="1" t="inlineStr"/>
-      <c r="K162" s="1" t="inlineStr"/>
-      <c r="L162" s="1" t="inlineStr"/>
-      <c r="M162" s="1" t="inlineStr"/>
-      <c r="N162" s="1" t="inlineStr"/>
-      <c r="O162" s="7" t="inlineStr"/>
-      <c r="P162" s="7" t="inlineStr"/>
-      <c r="Q162" s="7" t="inlineStr"/>
-      <c r="R162" s="1" t="inlineStr"/>
-      <c r="S162" s="1" t="inlineStr"/>
-    </row>
-    <row r="163" customHeight="1" ht="88">
-      <c r="A163" s="1" t="inlineStr"/>
-      <c r="B163" s="1" t="inlineStr"/>
-      <c r="C163" s="1" t="inlineStr"/>
-      <c r="D163" s="1" t="inlineStr"/>
-      <c r="E163" s="1" t="inlineStr"/>
-      <c r="F163" s="1" t="inlineStr"/>
-      <c r="G163" s="1" t="inlineStr"/>
-      <c r="H163" s="1" t="inlineStr"/>
-      <c r="I163" s="1" t="inlineStr"/>
-      <c r="J163" s="1" t="inlineStr"/>
-      <c r="K163" s="1" t="inlineStr"/>
-      <c r="L163" s="1" t="inlineStr"/>
-      <c r="M163" s="1" t="inlineStr"/>
-      <c r="N163" s="1" t="inlineStr"/>
-      <c r="O163" s="1" t="inlineStr"/>
-      <c r="P163" s="1" t="inlineStr"/>
-      <c r="Q163" s="1" t="inlineStr"/>
-      <c r="R163" s="1" t="inlineStr"/>
-      <c r="S163" s="1" t="inlineStr"/>
-    </row>
-    <row r="164" customHeight="1" ht="20">
-      <c r="A164" s="1" t="inlineStr"/>
-      <c r="B164" s="1" t="inlineStr"/>
-      <c r="C164" s="1" t="inlineStr"/>
-      <c r="D164" s="1" t="inlineStr"/>
-      <c r="E164" s="1" t="inlineStr"/>
-      <c r="F164" s="1" t="inlineStr"/>
-      <c r="G164" s="1" t="inlineStr"/>
-      <c r="H164" s="1" t="inlineStr"/>
-      <c r="I164" s="1" t="inlineStr"/>
-      <c r="J164" s="1" t="inlineStr"/>
-      <c r="K164" s="1" t="inlineStr"/>
-      <c r="L164" s="1" t="inlineStr"/>
-      <c r="M164" s="1" t="inlineStr"/>
-      <c r="N164" s="1" t="inlineStr"/>
-      <c r="O164" s="1" t="inlineStr"/>
-      <c r="P164" s="1" t="inlineStr"/>
-      <c r="Q164" s="1" t="inlineStr"/>
-      <c r="R164" s="1" t="inlineStr"/>
-      <c r="S164" s="1" t="inlineStr"/>
-    </row>
-    <row r="165" customHeight="1" ht="27">
-      <c r="A165" s="1" t="inlineStr"/>
-      <c r="B165" s="1" t="inlineStr"/>
-      <c r="C165" s="1" t="inlineStr"/>
-      <c r="D165" s="1" t="inlineStr"/>
-      <c r="E165" s="1" t="inlineStr"/>
-      <c r="F165" s="1" t="inlineStr"/>
-      <c r="G165" s="1" t="inlineStr"/>
-      <c r="H165" s="1" t="inlineStr"/>
-      <c r="I165" s="1" t="inlineStr"/>
-      <c r="J165" s="1" t="inlineStr"/>
-      <c r="K165" s="1" t="inlineStr"/>
-      <c r="L165" s="1" t="inlineStr"/>
-      <c r="M165" s="1" t="inlineStr"/>
-      <c r="N165" s="4" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">reg2</t>
-          </r>
-        </is>
-      </c>
-      <c r="O165" s="4" t="inlineStr"/>
-      <c r="P165" s="4" t="inlineStr"/>
-      <c r="Q165" s="4" t="inlineStr"/>
-      <c r="R165" s="1" t="inlineStr"/>
-      <c r="S165" s="1" t="inlineStr"/>
-    </row>
-    <row r="166" customHeight="1" ht="3">
-      <c r="A166" s="1" t="inlineStr"/>
-      <c r="B166" s="1" t="inlineStr"/>
-      <c r="C166" s="1" t="inlineStr"/>
-      <c r="D166" s="1" t="inlineStr"/>
-      <c r="E166" s="1" t="inlineStr"/>
-      <c r="F166" s="1" t="inlineStr"/>
-      <c r="G166" s="1" t="inlineStr"/>
-      <c r="H166" s="1" t="inlineStr"/>
-      <c r="I166" s="1" t="inlineStr"/>
-      <c r="J166" s="1" t="inlineStr"/>
-      <c r="K166" s="1" t="inlineStr"/>
-      <c r="L166" s="1" t="inlineStr"/>
-      <c r="M166" s="1" t="inlineStr"/>
-      <c r="N166" s="1" t="inlineStr"/>
-      <c r="O166" s="1" t="inlineStr"/>
-      <c r="P166" s="1" t="inlineStr"/>
-      <c r="Q166" s="1" t="inlineStr"/>
-      <c r="R166" s="1" t="inlineStr"/>
-      <c r="S166" s="1" t="inlineStr"/>
-    </row>
-    <row r="167" customHeight="1" ht="20">
-      <c r="A167" s="1" t="inlineStr"/>
-      <c r="B167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">التاريخ</t>
-          </r>
-        </is>
-      </c>
-      <c r="C167" s="5" t="inlineStr"/>
-      <c r="D167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ملاحظات</t>
-          </r>
-        </is>
-      </c>
-      <c r="E167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">الوجهة</t>
-          </r>
-        </is>
-      </c>
-      <c r="F167" s="5" t="inlineStr"/>
-      <c r="G167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">المصفاة</t>
-          </r>
-        </is>
-      </c>
-      <c r="H167" s="5" t="inlineStr"/>
-      <c r="I167" s="5" t="inlineStr"/>
-      <c r="J167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">المادة</t>
-          </r>
-        </is>
-      </c>
-      <c r="K167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">الكمية</t>
-          </r>
-        </is>
-      </c>
-      <c r="L167" s="5" t="inlineStr"/>
-      <c r="M167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">السائق</t>
-          </r>
-        </is>
-      </c>
-      <c r="N167" s="5" t="inlineStr"/>
-      <c r="O167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">المعرف</t>
-          </r>
-        </is>
-      </c>
-      <c r="P167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">المركبة</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q167" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">No</t>
-          </r>
-        </is>
-      </c>
-      <c r="R167" s="5" t="inlineStr"/>
-      <c r="S167" s="1" t="inlineStr"/>
-    </row>
-    <row r="168" customHeight="1" ht="5">
-      <c r="A168" s="1" t="inlineStr"/>
-      <c r="B168" s="1" t="inlineStr"/>
-      <c r="C168" s="1" t="inlineStr"/>
-      <c r="D168" s="1" t="inlineStr"/>
-      <c r="E168" s="1" t="inlineStr"/>
-      <c r="F168" s="1" t="inlineStr"/>
-      <c r="G168" s="1" t="inlineStr"/>
-      <c r="H168" s="1" t="inlineStr"/>
-      <c r="I168" s="1" t="inlineStr"/>
-      <c r="J168" s="1" t="inlineStr"/>
-      <c r="K168" s="1" t="inlineStr"/>
-      <c r="L168" s="1" t="inlineStr"/>
-      <c r="M168" s="1" t="inlineStr"/>
-      <c r="N168" s="1" t="inlineStr"/>
-      <c r="O168" s="1" t="inlineStr"/>
-      <c r="P168" s="1" t="inlineStr"/>
-      <c r="Q168" s="1" t="inlineStr"/>
-      <c r="R168" s="1" t="inlineStr"/>
-      <c r="S168" s="1" t="inlineStr"/>
-    </row>
-    <row r="169" customHeight="1" ht="1">
-      <c r="A169" s="1" t="inlineStr"/>
-      <c r="B169" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-05T00:31:39</t>
-          </r>
-        </is>
-      </c>
-      <c r="C169" s="6" t="inlineStr"/>
-      <c r="D169" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">b</t>
-          </r>
-        </is>
-      </c>
-      <c r="E169" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F169" s="7" t="inlineStr"/>
-      <c r="G169" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H169" s="7" t="inlineStr"/>
-      <c r="I169" s="7" t="inlineStr"/>
-      <c r="J169" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K169" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">36000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L169" s="7" t="inlineStr"/>
-      <c r="M169" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N169" s="7" t="inlineStr"/>
-      <c r="O169" s="1" t="inlineStr"/>
-      <c r="P169" s="1" t="inlineStr"/>
-      <c r="Q169" s="1" t="inlineStr"/>
-      <c r="R169" s="1" t="inlineStr"/>
-      <c r="S169" s="1" t="inlineStr"/>
-    </row>
-    <row r="170" customHeight="1" ht="29">
-      <c r="A170" s="1" t="inlineStr"/>
-      <c r="B170" s="6" t="inlineStr"/>
-      <c r="C170" s="6" t="inlineStr"/>
-      <c r="D170" s="7" t="inlineStr"/>
-      <c r="E170" s="7" t="inlineStr"/>
-      <c r="F170" s="7" t="inlineStr"/>
-      <c r="G170" s="7" t="inlineStr"/>
-      <c r="H170" s="7" t="inlineStr"/>
-      <c r="I170" s="7" t="inlineStr"/>
-      <c r="J170" s="7" t="inlineStr"/>
-      <c r="K170" s="7" t="inlineStr"/>
-      <c r="L170" s="7" t="inlineStr"/>
-      <c r="M170" s="7" t="inlineStr"/>
-      <c r="N170" s="7" t="inlineStr"/>
-      <c r="O170" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">52</t>
-          </r>
-        </is>
-      </c>
-      <c r="P170" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q170" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">52</t>
-          </r>
-        </is>
-      </c>
-      <c r="R170" s="1" t="inlineStr"/>
-      <c r="S170" s="1" t="inlineStr"/>
-    </row>
-    <row r="171" customHeight="1" ht="1">
-      <c r="A171" s="1" t="inlineStr"/>
-      <c r="B171" s="1" t="inlineStr"/>
-      <c r="C171" s="1" t="inlineStr"/>
-      <c r="D171" s="1" t="inlineStr"/>
-      <c r="E171" s="1" t="inlineStr"/>
-      <c r="F171" s="1" t="inlineStr"/>
-      <c r="G171" s="1" t="inlineStr"/>
-      <c r="H171" s="1" t="inlineStr"/>
-      <c r="I171" s="1" t="inlineStr"/>
-      <c r="J171" s="1" t="inlineStr"/>
-      <c r="K171" s="1" t="inlineStr"/>
-      <c r="L171" s="1" t="inlineStr"/>
-      <c r="M171" s="1" t="inlineStr"/>
-      <c r="N171" s="1" t="inlineStr"/>
-      <c r="O171" s="7" t="inlineStr"/>
-      <c r="P171" s="7" t="inlineStr"/>
-      <c r="Q171" s="7" t="inlineStr"/>
-      <c r="R171" s="1" t="inlineStr"/>
-      <c r="S171" s="1" t="inlineStr"/>
-    </row>
-    <row r="172" customHeight="1" ht="5">
-      <c r="A172" s="1" t="inlineStr"/>
-      <c r="B172" s="1" t="inlineStr"/>
-      <c r="C172" s="1" t="inlineStr"/>
-      <c r="D172" s="1" t="inlineStr"/>
-      <c r="E172" s="1" t="inlineStr"/>
-      <c r="F172" s="1" t="inlineStr"/>
-      <c r="G172" s="1" t="inlineStr"/>
-      <c r="H172" s="1" t="inlineStr"/>
-      <c r="I172" s="1" t="inlineStr"/>
-      <c r="J172" s="1" t="inlineStr"/>
-      <c r="K172" s="1" t="inlineStr"/>
-      <c r="L172" s="1" t="inlineStr"/>
-      <c r="M172" s="1" t="inlineStr"/>
-      <c r="N172" s="1" t="inlineStr"/>
-      <c r="O172" s="1" t="inlineStr"/>
-      <c r="P172" s="1" t="inlineStr"/>
-      <c r="Q172" s="1" t="inlineStr"/>
-      <c r="R172" s="1" t="inlineStr"/>
-      <c r="S172" s="1" t="inlineStr"/>
-    </row>
-    <row r="173" customHeight="1" ht="1">
-      <c r="A173" s="1" t="inlineStr"/>
-      <c r="B173" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-05T00:35:07</t>
-          </r>
-        </is>
-      </c>
-      <c r="C173" s="6" t="inlineStr"/>
-      <c r="D173" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">90</t>
-          </r>
-        </is>
-      </c>
-      <c r="E173" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F173" s="7" t="inlineStr"/>
-      <c r="G173" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H173" s="7" t="inlineStr"/>
-      <c r="I173" s="7" t="inlineStr"/>
-      <c r="J173" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K173" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">36000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L173" s="7" t="inlineStr"/>
-      <c r="M173" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N173" s="7" t="inlineStr"/>
-      <c r="O173" s="1" t="inlineStr"/>
-      <c r="P173" s="1" t="inlineStr"/>
-      <c r="Q173" s="1" t="inlineStr"/>
-      <c r="R173" s="1" t="inlineStr"/>
-      <c r="S173" s="1" t="inlineStr"/>
-    </row>
-    <row r="174" customHeight="1" ht="29">
-      <c r="A174" s="1" t="inlineStr"/>
-      <c r="B174" s="6" t="inlineStr"/>
-      <c r="C174" s="6" t="inlineStr"/>
-      <c r="D174" s="7" t="inlineStr"/>
-      <c r="E174" s="7" t="inlineStr"/>
-      <c r="F174" s="7" t="inlineStr"/>
-      <c r="G174" s="7" t="inlineStr"/>
-      <c r="H174" s="7" t="inlineStr"/>
-      <c r="I174" s="7" t="inlineStr"/>
-      <c r="J174" s="7" t="inlineStr"/>
-      <c r="K174" s="7" t="inlineStr"/>
-      <c r="L174" s="7" t="inlineStr"/>
-      <c r="M174" s="7" t="inlineStr"/>
-      <c r="N174" s="7" t="inlineStr"/>
-      <c r="O174" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">53</t>
-          </r>
-        </is>
-      </c>
-      <c r="P174" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q174" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">53</t>
-          </r>
-        </is>
-      </c>
-      <c r="R174" s="1" t="inlineStr"/>
-      <c r="S174" s="1" t="inlineStr"/>
-    </row>
-    <row r="175" customHeight="1" ht="1">
-      <c r="A175" s="1" t="inlineStr"/>
-      <c r="B175" s="1" t="inlineStr"/>
-      <c r="C175" s="1" t="inlineStr"/>
-      <c r="D175" s="1" t="inlineStr"/>
-      <c r="E175" s="1" t="inlineStr"/>
-      <c r="F175" s="1" t="inlineStr"/>
-      <c r="G175" s="1" t="inlineStr"/>
-      <c r="H175" s="1" t="inlineStr"/>
-      <c r="I175" s="1" t="inlineStr"/>
-      <c r="J175" s="1" t="inlineStr"/>
-      <c r="K175" s="1" t="inlineStr"/>
-      <c r="L175" s="1" t="inlineStr"/>
-      <c r="M175" s="1" t="inlineStr"/>
-      <c r="N175" s="1" t="inlineStr"/>
-      <c r="O175" s="7" t="inlineStr"/>
-      <c r="P175" s="7" t="inlineStr"/>
-      <c r="Q175" s="7" t="inlineStr"/>
-      <c r="R175" s="1" t="inlineStr"/>
-      <c r="S175" s="1" t="inlineStr"/>
-    </row>
-    <row r="176" customHeight="1" ht="5">
-      <c r="A176" s="1" t="inlineStr"/>
-      <c r="B176" s="1" t="inlineStr"/>
-      <c r="C176" s="1" t="inlineStr"/>
-      <c r="D176" s="1" t="inlineStr"/>
-      <c r="E176" s="1" t="inlineStr"/>
-      <c r="F176" s="1" t="inlineStr"/>
-      <c r="G176" s="1" t="inlineStr"/>
-      <c r="H176" s="1" t="inlineStr"/>
-      <c r="I176" s="1" t="inlineStr"/>
-      <c r="J176" s="1" t="inlineStr"/>
-      <c r="K176" s="1" t="inlineStr"/>
-      <c r="L176" s="1" t="inlineStr"/>
-      <c r="M176" s="1" t="inlineStr"/>
-      <c r="N176" s="1" t="inlineStr"/>
-      <c r="O176" s="1" t="inlineStr"/>
-      <c r="P176" s="1" t="inlineStr"/>
-      <c r="Q176" s="1" t="inlineStr"/>
-      <c r="R176" s="1" t="inlineStr"/>
-      <c r="S176" s="1" t="inlineStr"/>
-    </row>
-    <row r="177" customHeight="1" ht="1">
-      <c r="A177" s="1" t="inlineStr"/>
-      <c r="B177" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-05T20:56:37</t>
-          </r>
-        </is>
-      </c>
-      <c r="C177" s="6" t="inlineStr"/>
-      <c r="D177" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">cftyfyt</t>
-          </r>
-        </is>
-      </c>
-      <c r="E177" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F177" s="7" t="inlineStr"/>
-      <c r="G177" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H177" s="7" t="inlineStr"/>
-      <c r="I177" s="7" t="inlineStr"/>
-      <c r="J177" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K177" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">45000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L177" s="7" t="inlineStr"/>
-      <c r="M177" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">another</t>
-          </r>
-        </is>
-      </c>
-      <c r="N177" s="7" t="inlineStr"/>
-      <c r="O177" s="1" t="inlineStr"/>
-      <c r="P177" s="1" t="inlineStr"/>
-      <c r="Q177" s="1" t="inlineStr"/>
-      <c r="R177" s="1" t="inlineStr"/>
-      <c r="S177" s="1" t="inlineStr"/>
-    </row>
-    <row r="178" customHeight="1" ht="29">
-      <c r="A178" s="1" t="inlineStr"/>
-      <c r="B178" s="6" t="inlineStr"/>
-      <c r="C178" s="6" t="inlineStr"/>
-      <c r="D178" s="7" t="inlineStr"/>
-      <c r="E178" s="7" t="inlineStr"/>
-      <c r="F178" s="7" t="inlineStr"/>
-      <c r="G178" s="7" t="inlineStr"/>
-      <c r="H178" s="7" t="inlineStr"/>
-      <c r="I178" s="7" t="inlineStr"/>
-      <c r="J178" s="7" t="inlineStr"/>
-      <c r="K178" s="7" t="inlineStr"/>
-      <c r="L178" s="7" t="inlineStr"/>
-      <c r="M178" s="7" t="inlineStr"/>
-      <c r="N178" s="7" t="inlineStr"/>
-      <c r="O178" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">54</t>
-          </r>
-        </is>
-      </c>
-      <c r="P178" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">321654</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q178" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">54</t>
-          </r>
-        </is>
-      </c>
-      <c r="R178" s="1" t="inlineStr"/>
-      <c r="S178" s="1" t="inlineStr"/>
-    </row>
-    <row r="179" customHeight="1" ht="1">
-      <c r="A179" s="1" t="inlineStr"/>
-      <c r="B179" s="1" t="inlineStr"/>
-      <c r="C179" s="1" t="inlineStr"/>
-      <c r="D179" s="1" t="inlineStr"/>
-      <c r="E179" s="1" t="inlineStr"/>
-      <c r="F179" s="1" t="inlineStr"/>
-      <c r="G179" s="1" t="inlineStr"/>
-      <c r="H179" s="1" t="inlineStr"/>
-      <c r="I179" s="1" t="inlineStr"/>
-      <c r="J179" s="1" t="inlineStr"/>
-      <c r="K179" s="1" t="inlineStr"/>
-      <c r="L179" s="1" t="inlineStr"/>
-      <c r="M179" s="1" t="inlineStr"/>
-      <c r="N179" s="1" t="inlineStr"/>
-      <c r="O179" s="7" t="inlineStr"/>
-      <c r="P179" s="7" t="inlineStr"/>
-      <c r="Q179" s="7" t="inlineStr"/>
-      <c r="R179" s="1" t="inlineStr"/>
-      <c r="S179" s="1" t="inlineStr"/>
-    </row>
-    <row r="180" customHeight="1" ht="5">
-      <c r="A180" s="1" t="inlineStr"/>
-      <c r="B180" s="1" t="inlineStr"/>
-      <c r="C180" s="1" t="inlineStr"/>
-      <c r="D180" s="1" t="inlineStr"/>
-      <c r="E180" s="1" t="inlineStr"/>
-      <c r="F180" s="1" t="inlineStr"/>
-      <c r="G180" s="1" t="inlineStr"/>
-      <c r="H180" s="1" t="inlineStr"/>
-      <c r="I180" s="1" t="inlineStr"/>
-      <c r="J180" s="1" t="inlineStr"/>
-      <c r="K180" s="1" t="inlineStr"/>
-      <c r="L180" s="1" t="inlineStr"/>
-      <c r="M180" s="1" t="inlineStr"/>
-      <c r="N180" s="1" t="inlineStr"/>
-      <c r="O180" s="1" t="inlineStr"/>
-      <c r="P180" s="1" t="inlineStr"/>
-      <c r="Q180" s="1" t="inlineStr"/>
-      <c r="R180" s="1" t="inlineStr"/>
-      <c r="S180" s="1" t="inlineStr"/>
-    </row>
-    <row r="181" customHeight="1" ht="1">
-      <c r="A181" s="1" t="inlineStr"/>
-      <c r="B181" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-06T15:22:13</t>
-          </r>
-        </is>
-      </c>
-      <c r="C181" s="6" t="inlineStr"/>
-      <c r="D181" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">231</t>
-          </r>
-        </is>
-      </c>
-      <c r="E181" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F181" s="7" t="inlineStr"/>
-      <c r="G181" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H181" s="7" t="inlineStr"/>
-      <c r="I181" s="7" t="inlineStr"/>
-      <c r="J181" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat1</t>
-          </r>
-        </is>
-      </c>
-      <c r="K181" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">45000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L181" s="7" t="inlineStr"/>
-      <c r="M181" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">another</t>
-          </r>
-        </is>
-      </c>
-      <c r="N181" s="7" t="inlineStr"/>
-      <c r="O181" s="1" t="inlineStr"/>
-      <c r="P181" s="1" t="inlineStr"/>
-      <c r="Q181" s="1" t="inlineStr"/>
-      <c r="R181" s="1" t="inlineStr"/>
-      <c r="S181" s="1" t="inlineStr"/>
-    </row>
-    <row r="182" customHeight="1" ht="29">
-      <c r="A182" s="1" t="inlineStr"/>
-      <c r="B182" s="6" t="inlineStr"/>
-      <c r="C182" s="6" t="inlineStr"/>
-      <c r="D182" s="7" t="inlineStr"/>
-      <c r="E182" s="7" t="inlineStr"/>
-      <c r="F182" s="7" t="inlineStr"/>
-      <c r="G182" s="7" t="inlineStr"/>
-      <c r="H182" s="7" t="inlineStr"/>
-      <c r="I182" s="7" t="inlineStr"/>
-      <c r="J182" s="7" t="inlineStr"/>
-      <c r="K182" s="7" t="inlineStr"/>
-      <c r="L182" s="7" t="inlineStr"/>
-      <c r="M182" s="7" t="inlineStr"/>
-      <c r="N182" s="7" t="inlineStr"/>
-      <c r="O182" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">55</t>
-          </r>
-        </is>
-      </c>
-      <c r="P182" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">321654</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q182" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">58</t>
-          </r>
-        </is>
-      </c>
-      <c r="R182" s="1" t="inlineStr"/>
-      <c r="S182" s="1" t="inlineStr"/>
-    </row>
-    <row r="183" customHeight="1" ht="1">
-      <c r="A183" s="1" t="inlineStr"/>
-      <c r="B183" s="1" t="inlineStr"/>
-      <c r="C183" s="1" t="inlineStr"/>
-      <c r="D183" s="1" t="inlineStr"/>
-      <c r="E183" s="1" t="inlineStr"/>
-      <c r="F183" s="1" t="inlineStr"/>
-      <c r="G183" s="1" t="inlineStr"/>
-      <c r="H183" s="1" t="inlineStr"/>
-      <c r="I183" s="1" t="inlineStr"/>
-      <c r="J183" s="1" t="inlineStr"/>
-      <c r="K183" s="1" t="inlineStr"/>
-      <c r="L183" s="1" t="inlineStr"/>
-      <c r="M183" s="1" t="inlineStr"/>
-      <c r="N183" s="1" t="inlineStr"/>
-      <c r="O183" s="7" t="inlineStr"/>
-      <c r="P183" s="7" t="inlineStr"/>
-      <c r="Q183" s="7" t="inlineStr"/>
-      <c r="R183" s="1" t="inlineStr"/>
-      <c r="S183" s="1" t="inlineStr"/>
-    </row>
-    <row r="184" customHeight="1" ht="5">
-      <c r="A184" s="1" t="inlineStr"/>
-      <c r="B184" s="1" t="inlineStr"/>
-      <c r="C184" s="1" t="inlineStr"/>
-      <c r="D184" s="1" t="inlineStr"/>
-      <c r="E184" s="1" t="inlineStr"/>
-      <c r="F184" s="1" t="inlineStr"/>
-      <c r="G184" s="1" t="inlineStr"/>
-      <c r="H184" s="1" t="inlineStr"/>
-      <c r="I184" s="1" t="inlineStr"/>
-      <c r="J184" s="1" t="inlineStr"/>
-      <c r="K184" s="1" t="inlineStr"/>
-      <c r="L184" s="1" t="inlineStr"/>
-      <c r="M184" s="1" t="inlineStr"/>
-      <c r="N184" s="1" t="inlineStr"/>
-      <c r="O184" s="1" t="inlineStr"/>
-      <c r="P184" s="1" t="inlineStr"/>
-      <c r="Q184" s="1" t="inlineStr"/>
-      <c r="R184" s="1" t="inlineStr"/>
-      <c r="S184" s="1" t="inlineStr"/>
-    </row>
-    <row r="185" customHeight="1" ht="1">
-      <c r="A185" s="1" t="inlineStr"/>
-      <c r="B185" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-06T15:34:13</t>
-          </r>
-        </is>
-      </c>
-      <c r="C185" s="6" t="inlineStr"/>
-      <c r="D185" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2222</t>
-          </r>
-        </is>
-      </c>
-      <c r="E185" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F185" s="7" t="inlineStr"/>
-      <c r="G185" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H185" s="7" t="inlineStr"/>
-      <c r="I185" s="7" t="inlineStr"/>
-      <c r="J185" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K185" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">36000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L185" s="7" t="inlineStr"/>
-      <c r="M185" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N185" s="7" t="inlineStr"/>
-      <c r="O185" s="1" t="inlineStr"/>
-      <c r="P185" s="1" t="inlineStr"/>
-      <c r="Q185" s="1" t="inlineStr"/>
-      <c r="R185" s="1" t="inlineStr"/>
-      <c r="S185" s="1" t="inlineStr"/>
-    </row>
-    <row r="186" customHeight="1" ht="29">
-      <c r="A186" s="1" t="inlineStr"/>
-      <c r="B186" s="6" t="inlineStr"/>
-      <c r="C186" s="6" t="inlineStr"/>
-      <c r="D186" s="7" t="inlineStr"/>
-      <c r="E186" s="7" t="inlineStr"/>
-      <c r="F186" s="7" t="inlineStr"/>
-      <c r="G186" s="7" t="inlineStr"/>
-      <c r="H186" s="7" t="inlineStr"/>
-      <c r="I186" s="7" t="inlineStr"/>
-      <c r="J186" s="7" t="inlineStr"/>
-      <c r="K186" s="7" t="inlineStr"/>
-      <c r="L186" s="7" t="inlineStr"/>
-      <c r="M186" s="7" t="inlineStr"/>
-      <c r="N186" s="7" t="inlineStr"/>
-      <c r="O186" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">56</t>
-          </r>
-        </is>
-      </c>
-      <c r="P186" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q186" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">61</t>
-          </r>
-        </is>
-      </c>
-      <c r="R186" s="1" t="inlineStr"/>
-      <c r="S186" s="1" t="inlineStr"/>
-    </row>
-    <row r="187" customHeight="1" ht="1">
-      <c r="A187" s="1" t="inlineStr"/>
-      <c r="B187" s="1" t="inlineStr"/>
-      <c r="C187" s="1" t="inlineStr"/>
-      <c r="D187" s="1" t="inlineStr"/>
-      <c r="E187" s="1" t="inlineStr"/>
-      <c r="F187" s="1" t="inlineStr"/>
-      <c r="G187" s="1" t="inlineStr"/>
-      <c r="H187" s="1" t="inlineStr"/>
-      <c r="I187" s="1" t="inlineStr"/>
-      <c r="J187" s="1" t="inlineStr"/>
-      <c r="K187" s="1" t="inlineStr"/>
-      <c r="L187" s="1" t="inlineStr"/>
-      <c r="M187" s="1" t="inlineStr"/>
-      <c r="N187" s="1" t="inlineStr"/>
-      <c r="O187" s="7" t="inlineStr"/>
-      <c r="P187" s="7" t="inlineStr"/>
-      <c r="Q187" s="7" t="inlineStr"/>
-      <c r="R187" s="1" t="inlineStr"/>
-      <c r="S187" s="1" t="inlineStr"/>
-    </row>
-    <row r="188" customHeight="1" ht="5">
-      <c r="A188" s="1" t="inlineStr"/>
-      <c r="B188" s="1" t="inlineStr"/>
-      <c r="C188" s="1" t="inlineStr"/>
-      <c r="D188" s="1" t="inlineStr"/>
-      <c r="E188" s="1" t="inlineStr"/>
-      <c r="F188" s="1" t="inlineStr"/>
-      <c r="G188" s="1" t="inlineStr"/>
-      <c r="H188" s="1" t="inlineStr"/>
-      <c r="I188" s="1" t="inlineStr"/>
-      <c r="J188" s="1" t="inlineStr"/>
-      <c r="K188" s="1" t="inlineStr"/>
-      <c r="L188" s="1" t="inlineStr"/>
-      <c r="M188" s="1" t="inlineStr"/>
-      <c r="N188" s="1" t="inlineStr"/>
-      <c r="O188" s="1" t="inlineStr"/>
-      <c r="P188" s="1" t="inlineStr"/>
-      <c r="Q188" s="1" t="inlineStr"/>
-      <c r="R188" s="1" t="inlineStr"/>
-      <c r="S188" s="1" t="inlineStr"/>
-    </row>
-    <row r="189" customHeight="1" ht="1">
-      <c r="A189" s="1" t="inlineStr"/>
-      <c r="B189" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-11T14:32:28</t>
-          </r>
-        </is>
-      </c>
-      <c r="C189" s="6" t="inlineStr"/>
-      <c r="D189" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">w</t>
-          </r>
-        </is>
-      </c>
-      <c r="E189" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F189" s="7" t="inlineStr"/>
-      <c r="G189" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H189" s="7" t="inlineStr"/>
-      <c r="I189" s="7" t="inlineStr"/>
-      <c r="J189" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K189" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">30000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L189" s="7" t="inlineStr"/>
-      <c r="M189" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N189" s="7" t="inlineStr"/>
-      <c r="O189" s="1" t="inlineStr"/>
-      <c r="P189" s="1" t="inlineStr"/>
-      <c r="Q189" s="1" t="inlineStr"/>
-      <c r="R189" s="1" t="inlineStr"/>
-      <c r="S189" s="1" t="inlineStr"/>
-    </row>
-    <row r="190" customHeight="1" ht="29">
-      <c r="A190" s="1" t="inlineStr"/>
-      <c r="B190" s="6" t="inlineStr"/>
-      <c r="C190" s="6" t="inlineStr"/>
-      <c r="D190" s="7" t="inlineStr"/>
-      <c r="E190" s="7" t="inlineStr"/>
-      <c r="F190" s="7" t="inlineStr"/>
-      <c r="G190" s="7" t="inlineStr"/>
-      <c r="H190" s="7" t="inlineStr"/>
-      <c r="I190" s="7" t="inlineStr"/>
-      <c r="J190" s="7" t="inlineStr"/>
-      <c r="K190" s="7" t="inlineStr"/>
-      <c r="L190" s="7" t="inlineStr"/>
-      <c r="M190" s="7" t="inlineStr"/>
-      <c r="N190" s="7" t="inlineStr"/>
-      <c r="O190" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">71</t>
-          </r>
-        </is>
-      </c>
-      <c r="P190" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q190" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">91</t>
-          </r>
-        </is>
-      </c>
-      <c r="R190" s="1" t="inlineStr"/>
-      <c r="S190" s="1" t="inlineStr"/>
-    </row>
-    <row r="191" customHeight="1" ht="1">
-      <c r="A191" s="1" t="inlineStr"/>
-      <c r="B191" s="1" t="inlineStr"/>
-      <c r="C191" s="1" t="inlineStr"/>
-      <c r="D191" s="1" t="inlineStr"/>
-      <c r="E191" s="1" t="inlineStr"/>
-      <c r="F191" s="1" t="inlineStr"/>
-      <c r="G191" s="1" t="inlineStr"/>
-      <c r="H191" s="1" t="inlineStr"/>
-      <c r="I191" s="1" t="inlineStr"/>
-      <c r="J191" s="1" t="inlineStr"/>
-      <c r="K191" s="1" t="inlineStr"/>
-      <c r="L191" s="1" t="inlineStr"/>
-      <c r="M191" s="1" t="inlineStr"/>
-      <c r="N191" s="1" t="inlineStr"/>
-      <c r="O191" s="7" t="inlineStr"/>
-      <c r="P191" s="7" t="inlineStr"/>
-      <c r="Q191" s="7" t="inlineStr"/>
-      <c r="R191" s="1" t="inlineStr"/>
-      <c r="S191" s="1" t="inlineStr"/>
-    </row>
-    <row r="192" customHeight="1" ht="5">
-      <c r="A192" s="1" t="inlineStr"/>
-      <c r="B192" s="1" t="inlineStr"/>
-      <c r="C192" s="1" t="inlineStr"/>
-      <c r="D192" s="1" t="inlineStr"/>
-      <c r="E192" s="1" t="inlineStr"/>
-      <c r="F192" s="1" t="inlineStr"/>
-      <c r="G192" s="1" t="inlineStr"/>
-      <c r="H192" s="1" t="inlineStr"/>
-      <c r="I192" s="1" t="inlineStr"/>
-      <c r="J192" s="1" t="inlineStr"/>
-      <c r="K192" s="1" t="inlineStr"/>
-      <c r="L192" s="1" t="inlineStr"/>
-      <c r="M192" s="1" t="inlineStr"/>
-      <c r="N192" s="1" t="inlineStr"/>
-      <c r="O192" s="1" t="inlineStr"/>
-      <c r="P192" s="1" t="inlineStr"/>
-      <c r="Q192" s="1" t="inlineStr"/>
-      <c r="R192" s="1" t="inlineStr"/>
-      <c r="S192" s="1" t="inlineStr"/>
-    </row>
-    <row r="193" customHeight="1" ht="1">
-      <c r="A193" s="1" t="inlineStr"/>
-      <c r="B193" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-11T15:44:23</t>
-          </r>
-        </is>
-      </c>
-      <c r="C193" s="6" t="inlineStr"/>
-      <c r="D193" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">w</t>
-          </r>
-        </is>
-      </c>
-      <c r="E193" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F193" s="7" t="inlineStr"/>
-      <c r="G193" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H193" s="7" t="inlineStr"/>
-      <c r="I193" s="7" t="inlineStr"/>
-      <c r="J193" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K193" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">6000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L193" s="7" t="inlineStr"/>
-      <c r="M193" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N193" s="7" t="inlineStr"/>
-      <c r="O193" s="1" t="inlineStr"/>
-      <c r="P193" s="1" t="inlineStr"/>
-      <c r="Q193" s="1" t="inlineStr"/>
-      <c r="R193" s="1" t="inlineStr"/>
-      <c r="S193" s="1" t="inlineStr"/>
-    </row>
-    <row r="194" customHeight="1" ht="29">
-      <c r="A194" s="1" t="inlineStr"/>
-      <c r="B194" s="6" t="inlineStr"/>
-      <c r="C194" s="6" t="inlineStr"/>
-      <c r="D194" s="7" t="inlineStr"/>
-      <c r="E194" s="7" t="inlineStr"/>
-      <c r="F194" s="7" t="inlineStr"/>
-      <c r="G194" s="7" t="inlineStr"/>
-      <c r="H194" s="7" t="inlineStr"/>
-      <c r="I194" s="7" t="inlineStr"/>
-      <c r="J194" s="7" t="inlineStr"/>
-      <c r="K194" s="7" t="inlineStr"/>
-      <c r="L194" s="7" t="inlineStr"/>
-      <c r="M194" s="7" t="inlineStr"/>
-      <c r="N194" s="7" t="inlineStr"/>
-      <c r="O194" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">71</t>
-          </r>
-        </is>
-      </c>
-      <c r="P194" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q194" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">96</t>
-          </r>
-        </is>
-      </c>
-      <c r="R194" s="1" t="inlineStr"/>
-      <c r="S194" s="1" t="inlineStr"/>
-    </row>
-    <row r="195" customHeight="1" ht="1">
-      <c r="A195" s="1" t="inlineStr"/>
-      <c r="B195" s="1" t="inlineStr"/>
-      <c r="C195" s="1" t="inlineStr"/>
-      <c r="D195" s="1" t="inlineStr"/>
-      <c r="E195" s="1" t="inlineStr"/>
-      <c r="F195" s="1" t="inlineStr"/>
-      <c r="G195" s="1" t="inlineStr"/>
-      <c r="H195" s="1" t="inlineStr"/>
-      <c r="I195" s="1" t="inlineStr"/>
-      <c r="J195" s="1" t="inlineStr"/>
-      <c r="K195" s="1" t="inlineStr"/>
-      <c r="L195" s="1" t="inlineStr"/>
-      <c r="M195" s="1" t="inlineStr"/>
-      <c r="N195" s="1" t="inlineStr"/>
-      <c r="O195" s="7" t="inlineStr"/>
-      <c r="P195" s="7" t="inlineStr"/>
-      <c r="Q195" s="7" t="inlineStr"/>
-      <c r="R195" s="1" t="inlineStr"/>
-      <c r="S195" s="1" t="inlineStr"/>
-    </row>
-    <row r="196" customHeight="1" ht="5">
-      <c r="A196" s="1" t="inlineStr"/>
-      <c r="B196" s="1" t="inlineStr"/>
-      <c r="C196" s="1" t="inlineStr"/>
-      <c r="D196" s="1" t="inlineStr"/>
-      <c r="E196" s="1" t="inlineStr"/>
-      <c r="F196" s="1" t="inlineStr"/>
-      <c r="G196" s="1" t="inlineStr"/>
-      <c r="H196" s="1" t="inlineStr"/>
-      <c r="I196" s="1" t="inlineStr"/>
-      <c r="J196" s="1" t="inlineStr"/>
-      <c r="K196" s="1" t="inlineStr"/>
-      <c r="L196" s="1" t="inlineStr"/>
-      <c r="M196" s="1" t="inlineStr"/>
-      <c r="N196" s="1" t="inlineStr"/>
-      <c r="O196" s="1" t="inlineStr"/>
-      <c r="P196" s="1" t="inlineStr"/>
-      <c r="Q196" s="1" t="inlineStr"/>
-      <c r="R196" s="1" t="inlineStr"/>
-      <c r="S196" s="1" t="inlineStr"/>
-    </row>
-    <row r="197" customHeight="1" ht="1">
-      <c r="A197" s="1" t="inlineStr"/>
-      <c r="B197" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-11T16:04:50</t>
-          </r>
-        </is>
-      </c>
-      <c r="C197" s="6" t="inlineStr"/>
-      <c r="D197" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">56</t>
-          </r>
-        </is>
-      </c>
-      <c r="E197" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F197" s="7" t="inlineStr"/>
-      <c r="G197" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H197" s="7" t="inlineStr"/>
-      <c r="I197" s="7" t="inlineStr"/>
-      <c r="J197" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K197" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">36000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L197" s="7" t="inlineStr"/>
-      <c r="M197" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N197" s="7" t="inlineStr"/>
-      <c r="O197" s="1" t="inlineStr"/>
-      <c r="P197" s="1" t="inlineStr"/>
-      <c r="Q197" s="1" t="inlineStr"/>
-      <c r="R197" s="1" t="inlineStr"/>
-      <c r="S197" s="1" t="inlineStr"/>
-    </row>
-    <row r="198" customHeight="1" ht="29">
-      <c r="A198" s="1" t="inlineStr"/>
-      <c r="B198" s="6" t="inlineStr"/>
-      <c r="C198" s="6" t="inlineStr"/>
-      <c r="D198" s="7" t="inlineStr"/>
-      <c r="E198" s="7" t="inlineStr"/>
-      <c r="F198" s="7" t="inlineStr"/>
-      <c r="G198" s="7" t="inlineStr"/>
-      <c r="H198" s="7" t="inlineStr"/>
-      <c r="I198" s="7" t="inlineStr"/>
-      <c r="J198" s="7" t="inlineStr"/>
-      <c r="K198" s="7" t="inlineStr"/>
-      <c r="L198" s="7" t="inlineStr"/>
-      <c r="M198" s="7" t="inlineStr"/>
-      <c r="N198" s="7" t="inlineStr"/>
-      <c r="O198" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">72</t>
-          </r>
-        </is>
-      </c>
-      <c r="P198" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q198" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">102</t>
-          </r>
-        </is>
-      </c>
-      <c r="R198" s="1" t="inlineStr"/>
-      <c r="S198" s="1" t="inlineStr"/>
-    </row>
-    <row r="199" customHeight="1" ht="1">
-      <c r="A199" s="1" t="inlineStr"/>
-      <c r="B199" s="1" t="inlineStr"/>
-      <c r="C199" s="1" t="inlineStr"/>
-      <c r="D199" s="1" t="inlineStr"/>
-      <c r="E199" s="1" t="inlineStr"/>
-      <c r="F199" s="1" t="inlineStr"/>
-      <c r="G199" s="1" t="inlineStr"/>
-      <c r="H199" s="1" t="inlineStr"/>
-      <c r="I199" s="1" t="inlineStr"/>
-      <c r="J199" s="1" t="inlineStr"/>
-      <c r="K199" s="1" t="inlineStr"/>
-      <c r="L199" s="1" t="inlineStr"/>
-      <c r="M199" s="1" t="inlineStr"/>
-      <c r="N199" s="1" t="inlineStr"/>
-      <c r="O199" s="7" t="inlineStr"/>
-      <c r="P199" s="7" t="inlineStr"/>
-      <c r="Q199" s="7" t="inlineStr"/>
-      <c r="R199" s="1" t="inlineStr"/>
-      <c r="S199" s="1" t="inlineStr"/>
-    </row>
-    <row r="200" customHeight="1" ht="5">
-      <c r="A200" s="1" t="inlineStr"/>
-      <c r="B200" s="1" t="inlineStr"/>
-      <c r="C200" s="1" t="inlineStr"/>
-      <c r="D200" s="1" t="inlineStr"/>
-      <c r="E200" s="1" t="inlineStr"/>
-      <c r="F200" s="1" t="inlineStr"/>
-      <c r="G200" s="1" t="inlineStr"/>
-      <c r="H200" s="1" t="inlineStr"/>
-      <c r="I200" s="1" t="inlineStr"/>
-      <c r="J200" s="1" t="inlineStr"/>
-      <c r="K200" s="1" t="inlineStr"/>
-      <c r="L200" s="1" t="inlineStr"/>
-      <c r="M200" s="1" t="inlineStr"/>
-      <c r="N200" s="1" t="inlineStr"/>
-      <c r="O200" s="1" t="inlineStr"/>
-      <c r="P200" s="1" t="inlineStr"/>
-      <c r="Q200" s="1" t="inlineStr"/>
-      <c r="R200" s="1" t="inlineStr"/>
-      <c r="S200" s="1" t="inlineStr"/>
-    </row>
-    <row r="201" customHeight="1" ht="1">
-      <c r="A201" s="1" t="inlineStr"/>
-      <c r="B201" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-13T14:49:18</t>
-          </r>
-        </is>
-      </c>
-      <c r="C201" s="6" t="inlineStr"/>
-      <c r="D201" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">trt</t>
-          </r>
-        </is>
-      </c>
-      <c r="E201" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F201" s="7" t="inlineStr"/>
-      <c r="G201" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H201" s="7" t="inlineStr"/>
-      <c r="I201" s="7" t="inlineStr"/>
-      <c r="J201" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K201" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">36000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L201" s="7" t="inlineStr"/>
-      <c r="M201" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">pers</t>
-          </r>
-        </is>
-      </c>
-      <c r="N201" s="7" t="inlineStr"/>
-      <c r="O201" s="1" t="inlineStr"/>
-      <c r="P201" s="1" t="inlineStr"/>
-      <c r="Q201" s="1" t="inlineStr"/>
-      <c r="R201" s="1" t="inlineStr"/>
-      <c r="S201" s="1" t="inlineStr"/>
-    </row>
-    <row r="202" customHeight="1" ht="29">
-      <c r="A202" s="1" t="inlineStr"/>
-      <c r="B202" s="6" t="inlineStr"/>
-      <c r="C202" s="6" t="inlineStr"/>
-      <c r="D202" s="7" t="inlineStr"/>
-      <c r="E202" s="7" t="inlineStr"/>
-      <c r="F202" s="7" t="inlineStr"/>
-      <c r="G202" s="7" t="inlineStr"/>
-      <c r="H202" s="7" t="inlineStr"/>
-      <c r="I202" s="7" t="inlineStr"/>
-      <c r="J202" s="7" t="inlineStr"/>
-      <c r="K202" s="7" t="inlineStr"/>
-      <c r="L202" s="7" t="inlineStr"/>
-      <c r="M202" s="7" t="inlineStr"/>
-      <c r="N202" s="7" t="inlineStr"/>
-      <c r="O202" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">70</t>
-          </r>
-        </is>
-      </c>
-      <c r="P202" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">980980</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q202" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">103</t>
-          </r>
-        </is>
-      </c>
-      <c r="R202" s="1" t="inlineStr"/>
-      <c r="S202" s="1" t="inlineStr"/>
-    </row>
-    <row r="203" customHeight="1" ht="1">
-      <c r="A203" s="1" t="inlineStr"/>
-      <c r="B203" s="1" t="inlineStr"/>
-      <c r="C203" s="1" t="inlineStr"/>
-      <c r="D203" s="1" t="inlineStr"/>
-      <c r="E203" s="1" t="inlineStr"/>
-      <c r="F203" s="1" t="inlineStr"/>
-      <c r="G203" s="1" t="inlineStr"/>
-      <c r="H203" s="1" t="inlineStr"/>
-      <c r="I203" s="1" t="inlineStr"/>
-      <c r="J203" s="1" t="inlineStr"/>
-      <c r="K203" s="1" t="inlineStr"/>
-      <c r="L203" s="1" t="inlineStr"/>
-      <c r="M203" s="1" t="inlineStr"/>
-      <c r="N203" s="1" t="inlineStr"/>
-      <c r="O203" s="7" t="inlineStr"/>
-      <c r="P203" s="7" t="inlineStr"/>
-      <c r="Q203" s="7" t="inlineStr"/>
-      <c r="R203" s="1" t="inlineStr"/>
-      <c r="S203" s="1" t="inlineStr"/>
-    </row>
-    <row r="204" customHeight="1" ht="5">
-      <c r="A204" s="1" t="inlineStr"/>
-      <c r="B204" s="1" t="inlineStr"/>
-      <c r="C204" s="1" t="inlineStr"/>
-      <c r="D204" s="1" t="inlineStr"/>
-      <c r="E204" s="1" t="inlineStr"/>
-      <c r="F204" s="1" t="inlineStr"/>
-      <c r="G204" s="1" t="inlineStr"/>
-      <c r="H204" s="1" t="inlineStr"/>
-      <c r="I204" s="1" t="inlineStr"/>
-      <c r="J204" s="1" t="inlineStr"/>
-      <c r="K204" s="1" t="inlineStr"/>
-      <c r="L204" s="1" t="inlineStr"/>
-      <c r="M204" s="1" t="inlineStr"/>
-      <c r="N204" s="1" t="inlineStr"/>
-      <c r="O204" s="1" t="inlineStr"/>
-      <c r="P204" s="1" t="inlineStr"/>
-      <c r="Q204" s="1" t="inlineStr"/>
-      <c r="R204" s="1" t="inlineStr"/>
-      <c r="S204" s="1" t="inlineStr"/>
-    </row>
-    <row r="205" customHeight="1" ht="1">
-      <c r="A205" s="1" t="inlineStr"/>
-      <c r="B205" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-13T14:51:15</t>
-          </r>
-        </is>
-      </c>
-      <c r="C205" s="6" t="inlineStr"/>
-      <c r="D205" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">tttt</t>
-          </r>
-        </is>
-      </c>
-      <c r="E205" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F205" s="7" t="inlineStr"/>
-      <c r="G205" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H205" s="7" t="inlineStr"/>
-      <c r="I205" s="7" t="inlineStr"/>
-      <c r="J205" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K205" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">45000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L205" s="7" t="inlineStr"/>
-      <c r="M205" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">another</t>
-          </r>
-        </is>
-      </c>
-      <c r="N205" s="7" t="inlineStr"/>
-      <c r="O205" s="1" t="inlineStr"/>
-      <c r="P205" s="1" t="inlineStr"/>
-      <c r="Q205" s="1" t="inlineStr"/>
-      <c r="R205" s="1" t="inlineStr"/>
-      <c r="S205" s="1" t="inlineStr"/>
-    </row>
-    <row r="206" customHeight="1" ht="29">
-      <c r="A206" s="1" t="inlineStr"/>
-      <c r="B206" s="6" t="inlineStr"/>
-      <c r="C206" s="6" t="inlineStr"/>
-      <c r="D206" s="7" t="inlineStr"/>
-      <c r="E206" s="7" t="inlineStr"/>
-      <c r="F206" s="7" t="inlineStr"/>
-      <c r="G206" s="7" t="inlineStr"/>
-      <c r="H206" s="7" t="inlineStr"/>
-      <c r="I206" s="7" t="inlineStr"/>
-      <c r="J206" s="7" t="inlineStr"/>
-      <c r="K206" s="7" t="inlineStr"/>
-      <c r="L206" s="7" t="inlineStr"/>
-      <c r="M206" s="7" t="inlineStr"/>
-      <c r="N206" s="7" t="inlineStr"/>
-      <c r="O206" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">68</t>
-          </r>
-        </is>
-      </c>
-      <c r="P206" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">321654</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q206" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">104</t>
-          </r>
-        </is>
-      </c>
-      <c r="R206" s="1" t="inlineStr"/>
-      <c r="S206" s="1" t="inlineStr"/>
-    </row>
-    <row r="207" customHeight="1" ht="1">
-      <c r="A207" s="1" t="inlineStr"/>
-      <c r="B207" s="1" t="inlineStr"/>
-      <c r="C207" s="1" t="inlineStr"/>
-      <c r="D207" s="1" t="inlineStr"/>
-      <c r="E207" s="1" t="inlineStr"/>
-      <c r="F207" s="1" t="inlineStr"/>
-      <c r="G207" s="1" t="inlineStr"/>
-      <c r="H207" s="1" t="inlineStr"/>
-      <c r="I207" s="1" t="inlineStr"/>
-      <c r="J207" s="1" t="inlineStr"/>
-      <c r="K207" s="1" t="inlineStr"/>
-      <c r="L207" s="1" t="inlineStr"/>
-      <c r="M207" s="1" t="inlineStr"/>
-      <c r="N207" s="1" t="inlineStr"/>
-      <c r="O207" s="7" t="inlineStr"/>
-      <c r="P207" s="7" t="inlineStr"/>
-      <c r="Q207" s="7" t="inlineStr"/>
-      <c r="R207" s="1" t="inlineStr"/>
-      <c r="S207" s="1" t="inlineStr"/>
-    </row>
-    <row r="208" customHeight="1" ht="5">
-      <c r="A208" s="1" t="inlineStr"/>
-      <c r="B208" s="1" t="inlineStr"/>
-      <c r="C208" s="1" t="inlineStr"/>
-      <c r="D208" s="1" t="inlineStr"/>
-      <c r="E208" s="1" t="inlineStr"/>
-      <c r="F208" s="1" t="inlineStr"/>
-      <c r="G208" s="1" t="inlineStr"/>
-      <c r="H208" s="1" t="inlineStr"/>
-      <c r="I208" s="1" t="inlineStr"/>
-      <c r="J208" s="1" t="inlineStr"/>
-      <c r="K208" s="1" t="inlineStr"/>
-      <c r="L208" s="1" t="inlineStr"/>
-      <c r="M208" s="1" t="inlineStr"/>
-      <c r="N208" s="1" t="inlineStr"/>
-      <c r="O208" s="1" t="inlineStr"/>
-      <c r="P208" s="1" t="inlineStr"/>
-      <c r="Q208" s="1" t="inlineStr"/>
-      <c r="R208" s="1" t="inlineStr"/>
-      <c r="S208" s="1" t="inlineStr"/>
-    </row>
-    <row r="209" customHeight="1" ht="1">
-      <c r="A209" s="1" t="inlineStr"/>
-      <c r="B209" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-13T20:01:16</t>
-          </r>
-        </is>
-      </c>
-      <c r="C209" s="6" t="inlineStr"/>
-      <c r="D209" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">gt</t>
-          </r>
-        </is>
-      </c>
-      <c r="E209" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F209" s="7" t="inlineStr"/>
-      <c r="G209" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H209" s="7" t="inlineStr"/>
-      <c r="I209" s="7" t="inlineStr"/>
-      <c r="J209" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K209" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">45000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L209" s="7" t="inlineStr"/>
-      <c r="M209" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">another</t>
-          </r>
-        </is>
-      </c>
-      <c r="N209" s="7" t="inlineStr"/>
-      <c r="O209" s="1" t="inlineStr"/>
-      <c r="P209" s="1" t="inlineStr"/>
-      <c r="Q209" s="1" t="inlineStr"/>
-      <c r="R209" s="1" t="inlineStr"/>
-      <c r="S209" s="1" t="inlineStr"/>
-    </row>
-    <row r="210" customHeight="1" ht="29">
-      <c r="A210" s="1" t="inlineStr"/>
-      <c r="B210" s="6" t="inlineStr"/>
-      <c r="C210" s="6" t="inlineStr"/>
-      <c r="D210" s="7" t="inlineStr"/>
-      <c r="E210" s="7" t="inlineStr"/>
-      <c r="F210" s="7" t="inlineStr"/>
-      <c r="G210" s="7" t="inlineStr"/>
-      <c r="H210" s="7" t="inlineStr"/>
-      <c r="I210" s="7" t="inlineStr"/>
-      <c r="J210" s="7" t="inlineStr"/>
-      <c r="K210" s="7" t="inlineStr"/>
-      <c r="L210" s="7" t="inlineStr"/>
-      <c r="M210" s="7" t="inlineStr"/>
-      <c r="N210" s="7" t="inlineStr"/>
-      <c r="O210" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">73</t>
-          </r>
-        </is>
-      </c>
-      <c r="P210" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">321654</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q210" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">105</t>
-          </r>
-        </is>
-      </c>
-      <c r="R210" s="1" t="inlineStr"/>
-      <c r="S210" s="1" t="inlineStr"/>
-    </row>
-    <row r="211" customHeight="1" ht="1">
-      <c r="A211" s="1" t="inlineStr"/>
-      <c r="B211" s="1" t="inlineStr"/>
-      <c r="C211" s="1" t="inlineStr"/>
-      <c r="D211" s="1" t="inlineStr"/>
-      <c r="E211" s="1" t="inlineStr"/>
-      <c r="F211" s="1" t="inlineStr"/>
-      <c r="G211" s="1" t="inlineStr"/>
-      <c r="H211" s="1" t="inlineStr"/>
-      <c r="I211" s="1" t="inlineStr"/>
-      <c r="J211" s="1" t="inlineStr"/>
-      <c r="K211" s="1" t="inlineStr"/>
-      <c r="L211" s="1" t="inlineStr"/>
-      <c r="M211" s="1" t="inlineStr"/>
-      <c r="N211" s="1" t="inlineStr"/>
-      <c r="O211" s="7" t="inlineStr"/>
-      <c r="P211" s="7" t="inlineStr"/>
-      <c r="Q211" s="7" t="inlineStr"/>
-      <c r="R211" s="1" t="inlineStr"/>
-      <c r="S211" s="1" t="inlineStr"/>
-    </row>
-    <row r="212" customHeight="1" ht="5">
-      <c r="A212" s="1" t="inlineStr"/>
-      <c r="B212" s="1" t="inlineStr"/>
-      <c r="C212" s="1" t="inlineStr"/>
-      <c r="D212" s="1" t="inlineStr"/>
-      <c r="E212" s="1" t="inlineStr"/>
-      <c r="F212" s="1" t="inlineStr"/>
-      <c r="G212" s="1" t="inlineStr"/>
-      <c r="H212" s="1" t="inlineStr"/>
-      <c r="I212" s="1" t="inlineStr"/>
-      <c r="J212" s="1" t="inlineStr"/>
-      <c r="K212" s="1" t="inlineStr"/>
-      <c r="L212" s="1" t="inlineStr"/>
-      <c r="M212" s="1" t="inlineStr"/>
-      <c r="N212" s="1" t="inlineStr"/>
-      <c r="O212" s="1" t="inlineStr"/>
-      <c r="P212" s="1" t="inlineStr"/>
-      <c r="Q212" s="1" t="inlineStr"/>
-      <c r="R212" s="1" t="inlineStr"/>
-      <c r="S212" s="1" t="inlineStr"/>
-    </row>
-    <row r="213" customHeight="1" ht="1">
-      <c r="A213" s="1" t="inlineStr"/>
-      <c r="B213" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">2023-11-13T20:02:07</t>
-          </r>
-        </is>
-      </c>
-      <c r="C213" s="6" t="inlineStr"/>
-      <c r="D213" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">55</t>
-          </r>
-        </is>
-      </c>
-      <c r="E213" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">myTest</t>
-          </r>
-        </is>
-      </c>
-      <c r="F213" s="7" t="inlineStr"/>
-      <c r="G213" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ref1</t>
-          </r>
-        </is>
-      </c>
-      <c r="H213" s="7" t="inlineStr"/>
-      <c r="I213" s="7" t="inlineStr"/>
-      <c r="J213" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">mat2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K213" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">45000</t>
-          </r>
-        </is>
-      </c>
-      <c r="L213" s="7" t="inlineStr"/>
-      <c r="M213" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">another</t>
-          </r>
-        </is>
-      </c>
-      <c r="N213" s="7" t="inlineStr"/>
-      <c r="O213" s="1" t="inlineStr"/>
-      <c r="P213" s="1" t="inlineStr"/>
-      <c r="Q213" s="1" t="inlineStr"/>
-      <c r="R213" s="1" t="inlineStr"/>
-      <c r="S213" s="1" t="inlineStr"/>
-    </row>
-    <row r="214" customHeight="1" ht="29">
-      <c r="A214" s="1" t="inlineStr"/>
-      <c r="B214" s="6" t="inlineStr"/>
-      <c r="C214" s="6" t="inlineStr"/>
-      <c r="D214" s="7" t="inlineStr"/>
-      <c r="E214" s="7" t="inlineStr"/>
-      <c r="F214" s="7" t="inlineStr"/>
-      <c r="G214" s="7" t="inlineStr"/>
-      <c r="H214" s="7" t="inlineStr"/>
-      <c r="I214" s="7" t="inlineStr"/>
-      <c r="J214" s="7" t="inlineStr"/>
-      <c r="K214" s="7" t="inlineStr"/>
-      <c r="L214" s="7" t="inlineStr"/>
-      <c r="M214" s="7" t="inlineStr"/>
-      <c r="N214" s="7" t="inlineStr"/>
-      <c r="O214" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">74</t>
-          </r>
-        </is>
-      </c>
-      <c r="P214" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">321654</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q214" s="7" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">106</t>
-          </r>
-        </is>
-      </c>
-      <c r="R214" s="1" t="inlineStr"/>
-      <c r="S214" s="1" t="inlineStr"/>
-    </row>
-    <row r="215" customHeight="1" ht="1">
-      <c r="A215" s="1" t="inlineStr"/>
-      <c r="B215" s="1" t="inlineStr"/>
-      <c r="C215" s="1" t="inlineStr"/>
-      <c r="D215" s="1" t="inlineStr"/>
-      <c r="E215" s="1" t="inlineStr"/>
-      <c r="F215" s="1" t="inlineStr"/>
-      <c r="G215" s="1" t="inlineStr"/>
-      <c r="H215" s="1" t="inlineStr"/>
-      <c r="I215" s="1" t="inlineStr"/>
-      <c r="J215" s="1" t="inlineStr"/>
-      <c r="K215" s="1" t="inlineStr"/>
-      <c r="L215" s="1" t="inlineStr"/>
-      <c r="M215" s="1" t="inlineStr"/>
-      <c r="N215" s="1" t="inlineStr"/>
-      <c r="O215" s="7" t="inlineStr"/>
-      <c r="P215" s="7" t="inlineStr"/>
-      <c r="Q215" s="7" t="inlineStr"/>
-      <c r="R215" s="1" t="inlineStr"/>
-      <c r="S215" s="1" t="inlineStr"/>
-    </row>
-    <row r="216" customHeight="1" ht="340">
-      <c r="A216" s="1" t="inlineStr"/>
-      <c r="B216" s="1" t="inlineStr"/>
-      <c r="C216" s="1" t="inlineStr"/>
-      <c r="D216" s="1" t="inlineStr"/>
-      <c r="E216" s="1" t="inlineStr"/>
-      <c r="F216" s="1" t="inlineStr"/>
-      <c r="G216" s="1" t="inlineStr"/>
-      <c r="H216" s="1" t="inlineStr"/>
-      <c r="I216" s="1" t="inlineStr"/>
-      <c r="J216" s="1" t="inlineStr"/>
-      <c r="K216" s="1" t="inlineStr"/>
-      <c r="L216" s="1" t="inlineStr"/>
-      <c r="M216" s="1" t="inlineStr"/>
-      <c r="N216" s="1" t="inlineStr"/>
-      <c r="O216" s="1" t="inlineStr"/>
-      <c r="P216" s="1" t="inlineStr"/>
-      <c r="Q216" s="1" t="inlineStr"/>
-      <c r="R216" s="1" t="inlineStr"/>
-      <c r="S216" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -8303,153 +6116,6 @@
     <mergeCell ref="O153:O154"/>
     <mergeCell ref="P153:P154"/>
     <mergeCell ref="Q153:Q154"/>
-    <mergeCell ref="B156:C157"/>
-    <mergeCell ref="D156:D157"/>
-    <mergeCell ref="E156:F157"/>
-    <mergeCell ref="G156:I157"/>
-    <mergeCell ref="J156:J157"/>
-    <mergeCell ref="K156:L157"/>
-    <mergeCell ref="M156:N157"/>
-    <mergeCell ref="O157:O158"/>
-    <mergeCell ref="P157:P158"/>
-    <mergeCell ref="Q157:Q158"/>
-    <mergeCell ref="B160:C161"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="E160:F161"/>
-    <mergeCell ref="G160:I161"/>
-    <mergeCell ref="J160:J161"/>
-    <mergeCell ref="K160:L161"/>
-    <mergeCell ref="M160:N161"/>
-    <mergeCell ref="O161:O162"/>
-    <mergeCell ref="P161:P162"/>
-    <mergeCell ref="Q161:Q162"/>
-    <mergeCell ref="N165:Q165"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="E167:F167"/>
-    <mergeCell ref="G167:I167"/>
-    <mergeCell ref="K167:L167"/>
-    <mergeCell ref="M167:N167"/>
-    <mergeCell ref="Q167:R167"/>
-    <mergeCell ref="B169:C170"/>
-    <mergeCell ref="D169:D170"/>
-    <mergeCell ref="E169:F170"/>
-    <mergeCell ref="G169:I170"/>
-    <mergeCell ref="J169:J170"/>
-    <mergeCell ref="K169:L170"/>
-    <mergeCell ref="M169:N170"/>
-    <mergeCell ref="O170:O171"/>
-    <mergeCell ref="P170:P171"/>
-    <mergeCell ref="Q170:Q171"/>
-    <mergeCell ref="B173:C174"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="E173:F174"/>
-    <mergeCell ref="G173:I174"/>
-    <mergeCell ref="J173:J174"/>
-    <mergeCell ref="K173:L174"/>
-    <mergeCell ref="M173:N174"/>
-    <mergeCell ref="O174:O175"/>
-    <mergeCell ref="P174:P175"/>
-    <mergeCell ref="Q174:Q175"/>
-    <mergeCell ref="B177:C178"/>
-    <mergeCell ref="D177:D178"/>
-    <mergeCell ref="E177:F178"/>
-    <mergeCell ref="G177:I178"/>
-    <mergeCell ref="J177:J178"/>
-    <mergeCell ref="K177:L178"/>
-    <mergeCell ref="M177:N178"/>
-    <mergeCell ref="O178:O179"/>
-    <mergeCell ref="P178:P179"/>
-    <mergeCell ref="Q178:Q179"/>
-    <mergeCell ref="B181:C182"/>
-    <mergeCell ref="D181:D182"/>
-    <mergeCell ref="E181:F182"/>
-    <mergeCell ref="G181:I182"/>
-    <mergeCell ref="J181:J182"/>
-    <mergeCell ref="K181:L182"/>
-    <mergeCell ref="M181:N182"/>
-    <mergeCell ref="O182:O183"/>
-    <mergeCell ref="P182:P183"/>
-    <mergeCell ref="Q182:Q183"/>
-    <mergeCell ref="B185:C186"/>
-    <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E185:F186"/>
-    <mergeCell ref="G185:I186"/>
-    <mergeCell ref="J185:J186"/>
-    <mergeCell ref="K185:L186"/>
-    <mergeCell ref="M185:N186"/>
-    <mergeCell ref="O186:O187"/>
-    <mergeCell ref="P186:P187"/>
-    <mergeCell ref="Q186:Q187"/>
-    <mergeCell ref="B189:C190"/>
-    <mergeCell ref="D189:D190"/>
-    <mergeCell ref="E189:F190"/>
-    <mergeCell ref="G189:I190"/>
-    <mergeCell ref="J189:J190"/>
-    <mergeCell ref="K189:L190"/>
-    <mergeCell ref="M189:N190"/>
-    <mergeCell ref="O190:O191"/>
-    <mergeCell ref="P190:P191"/>
-    <mergeCell ref="Q190:Q191"/>
-    <mergeCell ref="B193:C194"/>
-    <mergeCell ref="D193:D194"/>
-    <mergeCell ref="E193:F194"/>
-    <mergeCell ref="G193:I194"/>
-    <mergeCell ref="J193:J194"/>
-    <mergeCell ref="K193:L194"/>
-    <mergeCell ref="M193:N194"/>
-    <mergeCell ref="O194:O195"/>
-    <mergeCell ref="P194:P195"/>
-    <mergeCell ref="Q194:Q195"/>
-    <mergeCell ref="B197:C198"/>
-    <mergeCell ref="D197:D198"/>
-    <mergeCell ref="E197:F198"/>
-    <mergeCell ref="G197:I198"/>
-    <mergeCell ref="J197:J198"/>
-    <mergeCell ref="K197:L198"/>
-    <mergeCell ref="M197:N198"/>
-    <mergeCell ref="O198:O199"/>
-    <mergeCell ref="P198:P199"/>
-    <mergeCell ref="Q198:Q199"/>
-    <mergeCell ref="B201:C202"/>
-    <mergeCell ref="D201:D202"/>
-    <mergeCell ref="E201:F202"/>
-    <mergeCell ref="G201:I202"/>
-    <mergeCell ref="J201:J202"/>
-    <mergeCell ref="K201:L202"/>
-    <mergeCell ref="M201:N202"/>
-    <mergeCell ref="O202:O203"/>
-    <mergeCell ref="P202:P203"/>
-    <mergeCell ref="Q202:Q203"/>
-    <mergeCell ref="B205:C206"/>
-    <mergeCell ref="D205:D206"/>
-    <mergeCell ref="E205:F206"/>
-    <mergeCell ref="G205:I206"/>
-    <mergeCell ref="J205:J206"/>
-    <mergeCell ref="K205:L206"/>
-    <mergeCell ref="M205:N206"/>
-    <mergeCell ref="O206:O207"/>
-    <mergeCell ref="P206:P207"/>
-    <mergeCell ref="Q206:Q207"/>
-    <mergeCell ref="B209:C210"/>
-    <mergeCell ref="D209:D210"/>
-    <mergeCell ref="E209:F210"/>
-    <mergeCell ref="G209:I210"/>
-    <mergeCell ref="J209:J210"/>
-    <mergeCell ref="K209:L210"/>
-    <mergeCell ref="M209:N210"/>
-    <mergeCell ref="O210:O211"/>
-    <mergeCell ref="P210:P211"/>
-    <mergeCell ref="Q210:Q211"/>
-    <mergeCell ref="B213:C214"/>
-    <mergeCell ref="D213:D214"/>
-    <mergeCell ref="E213:F214"/>
-    <mergeCell ref="G213:I214"/>
-    <mergeCell ref="J213:J214"/>
-    <mergeCell ref="K213:L214"/>
-    <mergeCell ref="M213:N214"/>
-    <mergeCell ref="O214:O215"/>
-    <mergeCell ref="P214:P215"/>
-    <mergeCell ref="Q214:Q215"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.00" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Base64 decode for report binary data
</commit_message>
<xml_diff>
--- a/Service/src/main/resources/templates/regionReport.xlsx
+++ b/Service/src/main/resources/templates/regionReport.xlsx
@@ -324,7 +324,7 @@
       <c r="C4" s="3" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2023-11-26T19:35:16</t>
+            <t xml:space="preserve">2023-12-16T13:11:47</t>
           </r>
         </is>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="R154" s="1" t="inlineStr"/>
       <c r="S154" s="1" t="inlineStr"/>
     </row>
-    <row r="155" customHeight="1" ht="160">
+    <row r="155" customHeight="1" ht="5">
       <c r="A155" s="1" t="inlineStr"/>
       <c r="B155" s="1" t="inlineStr"/>
       <c r="C155" s="1" t="inlineStr"/>
@@ -5747,6 +5747,1329 @@
       <c r="Q155" s="1" t="inlineStr"/>
       <c r="R155" s="1" t="inlineStr"/>
       <c r="S155" s="1" t="inlineStr"/>
+    </row>
+    <row r="156" customHeight="1" ht="1">
+      <c r="A156" s="1" t="inlineStr"/>
+      <c r="B156" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-06T15:22:13</t>
+          </r>
+        </is>
+      </c>
+      <c r="C156" s="6" t="inlineStr"/>
+      <c r="D156" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">231</t>
+          </r>
+        </is>
+      </c>
+      <c r="E156" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F156" s="7" t="inlineStr"/>
+      <c r="G156" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H156" s="7" t="inlineStr"/>
+      <c r="I156" s="7" t="inlineStr"/>
+      <c r="J156" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat1</t>
+          </r>
+        </is>
+      </c>
+      <c r="K156" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">45000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L156" s="7" t="inlineStr"/>
+      <c r="M156" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">another</t>
+          </r>
+        </is>
+      </c>
+      <c r="N156" s="7" t="inlineStr"/>
+      <c r="O156" s="1" t="inlineStr"/>
+      <c r="P156" s="1" t="inlineStr"/>
+      <c r="Q156" s="1" t="inlineStr"/>
+      <c r="R156" s="1" t="inlineStr"/>
+      <c r="S156" s="1" t="inlineStr"/>
+    </row>
+    <row r="157" customHeight="1" ht="29">
+      <c r="A157" s="1" t="inlineStr"/>
+      <c r="B157" s="6" t="inlineStr"/>
+      <c r="C157" s="6" t="inlineStr"/>
+      <c r="D157" s="7" t="inlineStr"/>
+      <c r="E157" s="7" t="inlineStr"/>
+      <c r="F157" s="7" t="inlineStr"/>
+      <c r="G157" s="7" t="inlineStr"/>
+      <c r="H157" s="7" t="inlineStr"/>
+      <c r="I157" s="7" t="inlineStr"/>
+      <c r="J157" s="7" t="inlineStr"/>
+      <c r="K157" s="7" t="inlineStr"/>
+      <c r="L157" s="7" t="inlineStr"/>
+      <c r="M157" s="7" t="inlineStr"/>
+      <c r="N157" s="7" t="inlineStr"/>
+      <c r="O157" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">55</t>
+          </r>
+        </is>
+      </c>
+      <c r="P157" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">321654</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q157" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">58</t>
+          </r>
+        </is>
+      </c>
+      <c r="R157" s="1" t="inlineStr"/>
+      <c r="S157" s="1" t="inlineStr"/>
+    </row>
+    <row r="158" customHeight="1" ht="1">
+      <c r="A158" s="1" t="inlineStr"/>
+      <c r="B158" s="1" t="inlineStr"/>
+      <c r="C158" s="1" t="inlineStr"/>
+      <c r="D158" s="1" t="inlineStr"/>
+      <c r="E158" s="1" t="inlineStr"/>
+      <c r="F158" s="1" t="inlineStr"/>
+      <c r="G158" s="1" t="inlineStr"/>
+      <c r="H158" s="1" t="inlineStr"/>
+      <c r="I158" s="1" t="inlineStr"/>
+      <c r="J158" s="1" t="inlineStr"/>
+      <c r="K158" s="1" t="inlineStr"/>
+      <c r="L158" s="1" t="inlineStr"/>
+      <c r="M158" s="1" t="inlineStr"/>
+      <c r="N158" s="1" t="inlineStr"/>
+      <c r="O158" s="7" t="inlineStr"/>
+      <c r="P158" s="7" t="inlineStr"/>
+      <c r="Q158" s="7" t="inlineStr"/>
+      <c r="R158" s="1" t="inlineStr"/>
+      <c r="S158" s="1" t="inlineStr"/>
+    </row>
+    <row r="159" customHeight="1" ht="5">
+      <c r="A159" s="1" t="inlineStr"/>
+      <c r="B159" s="1" t="inlineStr"/>
+      <c r="C159" s="1" t="inlineStr"/>
+      <c r="D159" s="1" t="inlineStr"/>
+      <c r="E159" s="1" t="inlineStr"/>
+      <c r="F159" s="1" t="inlineStr"/>
+      <c r="G159" s="1" t="inlineStr"/>
+      <c r="H159" s="1" t="inlineStr"/>
+      <c r="I159" s="1" t="inlineStr"/>
+      <c r="J159" s="1" t="inlineStr"/>
+      <c r="K159" s="1" t="inlineStr"/>
+      <c r="L159" s="1" t="inlineStr"/>
+      <c r="M159" s="1" t="inlineStr"/>
+      <c r="N159" s="1" t="inlineStr"/>
+      <c r="O159" s="1" t="inlineStr"/>
+      <c r="P159" s="1" t="inlineStr"/>
+      <c r="Q159" s="1" t="inlineStr"/>
+      <c r="R159" s="1" t="inlineStr"/>
+      <c r="S159" s="1" t="inlineStr"/>
+    </row>
+    <row r="160" customHeight="1" ht="1">
+      <c r="A160" s="1" t="inlineStr"/>
+      <c r="B160" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-06T15:34:13</t>
+          </r>
+        </is>
+      </c>
+      <c r="C160" s="6" t="inlineStr"/>
+      <c r="D160" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2222</t>
+          </r>
+        </is>
+      </c>
+      <c r="E160" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F160" s="7" t="inlineStr"/>
+      <c r="G160" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H160" s="7" t="inlineStr"/>
+      <c r="I160" s="7" t="inlineStr"/>
+      <c r="J160" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K160" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">36000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L160" s="7" t="inlineStr"/>
+      <c r="M160" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">pers</t>
+          </r>
+        </is>
+      </c>
+      <c r="N160" s="7" t="inlineStr"/>
+      <c r="O160" s="1" t="inlineStr"/>
+      <c r="P160" s="1" t="inlineStr"/>
+      <c r="Q160" s="1" t="inlineStr"/>
+      <c r="R160" s="1" t="inlineStr"/>
+      <c r="S160" s="1" t="inlineStr"/>
+    </row>
+    <row r="161" customHeight="1" ht="29">
+      <c r="A161" s="1" t="inlineStr"/>
+      <c r="B161" s="6" t="inlineStr"/>
+      <c r="C161" s="6" t="inlineStr"/>
+      <c r="D161" s="7" t="inlineStr"/>
+      <c r="E161" s="7" t="inlineStr"/>
+      <c r="F161" s="7" t="inlineStr"/>
+      <c r="G161" s="7" t="inlineStr"/>
+      <c r="H161" s="7" t="inlineStr"/>
+      <c r="I161" s="7" t="inlineStr"/>
+      <c r="J161" s="7" t="inlineStr"/>
+      <c r="K161" s="7" t="inlineStr"/>
+      <c r="L161" s="7" t="inlineStr"/>
+      <c r="M161" s="7" t="inlineStr"/>
+      <c r="N161" s="7" t="inlineStr"/>
+      <c r="O161" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">56</t>
+          </r>
+        </is>
+      </c>
+      <c r="P161" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">980980</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q161" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">61</t>
+          </r>
+        </is>
+      </c>
+      <c r="R161" s="1" t="inlineStr"/>
+      <c r="S161" s="1" t="inlineStr"/>
+    </row>
+    <row r="162" customHeight="1" ht="1">
+      <c r="A162" s="1" t="inlineStr"/>
+      <c r="B162" s="1" t="inlineStr"/>
+      <c r="C162" s="1" t="inlineStr"/>
+      <c r="D162" s="1" t="inlineStr"/>
+      <c r="E162" s="1" t="inlineStr"/>
+      <c r="F162" s="1" t="inlineStr"/>
+      <c r="G162" s="1" t="inlineStr"/>
+      <c r="H162" s="1" t="inlineStr"/>
+      <c r="I162" s="1" t="inlineStr"/>
+      <c r="J162" s="1" t="inlineStr"/>
+      <c r="K162" s="1" t="inlineStr"/>
+      <c r="L162" s="1" t="inlineStr"/>
+      <c r="M162" s="1" t="inlineStr"/>
+      <c r="N162" s="1" t="inlineStr"/>
+      <c r="O162" s="7" t="inlineStr"/>
+      <c r="P162" s="7" t="inlineStr"/>
+      <c r="Q162" s="7" t="inlineStr"/>
+      <c r="R162" s="1" t="inlineStr"/>
+      <c r="S162" s="1" t="inlineStr"/>
+    </row>
+    <row r="163" customHeight="1" ht="88">
+      <c r="A163" s="1" t="inlineStr"/>
+      <c r="B163" s="1" t="inlineStr"/>
+      <c r="C163" s="1" t="inlineStr"/>
+      <c r="D163" s="1" t="inlineStr"/>
+      <c r="E163" s="1" t="inlineStr"/>
+      <c r="F163" s="1" t="inlineStr"/>
+      <c r="G163" s="1" t="inlineStr"/>
+      <c r="H163" s="1" t="inlineStr"/>
+      <c r="I163" s="1" t="inlineStr"/>
+      <c r="J163" s="1" t="inlineStr"/>
+      <c r="K163" s="1" t="inlineStr"/>
+      <c r="L163" s="1" t="inlineStr"/>
+      <c r="M163" s="1" t="inlineStr"/>
+      <c r="N163" s="1" t="inlineStr"/>
+      <c r="O163" s="1" t="inlineStr"/>
+      <c r="P163" s="1" t="inlineStr"/>
+      <c r="Q163" s="1" t="inlineStr"/>
+      <c r="R163" s="1" t="inlineStr"/>
+      <c r="S163" s="1" t="inlineStr"/>
+    </row>
+    <row r="164" customHeight="1" ht="20">
+      <c r="A164" s="1" t="inlineStr"/>
+      <c r="B164" s="1" t="inlineStr"/>
+      <c r="C164" s="1" t="inlineStr"/>
+      <c r="D164" s="1" t="inlineStr"/>
+      <c r="E164" s="1" t="inlineStr"/>
+      <c r="F164" s="1" t="inlineStr"/>
+      <c r="G164" s="1" t="inlineStr"/>
+      <c r="H164" s="1" t="inlineStr"/>
+      <c r="I164" s="1" t="inlineStr"/>
+      <c r="J164" s="1" t="inlineStr"/>
+      <c r="K164" s="1" t="inlineStr"/>
+      <c r="L164" s="1" t="inlineStr"/>
+      <c r="M164" s="1" t="inlineStr"/>
+      <c r="N164" s="1" t="inlineStr"/>
+      <c r="O164" s="1" t="inlineStr"/>
+      <c r="P164" s="1" t="inlineStr"/>
+      <c r="Q164" s="1" t="inlineStr"/>
+      <c r="R164" s="1" t="inlineStr"/>
+      <c r="S164" s="1" t="inlineStr"/>
+    </row>
+    <row r="165" customHeight="1" ht="27">
+      <c r="A165" s="1" t="inlineStr"/>
+      <c r="B165" s="1" t="inlineStr"/>
+      <c r="C165" s="1" t="inlineStr"/>
+      <c r="D165" s="1" t="inlineStr"/>
+      <c r="E165" s="1" t="inlineStr"/>
+      <c r="F165" s="1" t="inlineStr"/>
+      <c r="G165" s="1" t="inlineStr"/>
+      <c r="H165" s="1" t="inlineStr"/>
+      <c r="I165" s="1" t="inlineStr"/>
+      <c r="J165" s="1" t="inlineStr"/>
+      <c r="K165" s="1" t="inlineStr"/>
+      <c r="L165" s="1" t="inlineStr"/>
+      <c r="M165" s="1" t="inlineStr"/>
+      <c r="N165" s="4" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">reg2</t>
+          </r>
+        </is>
+      </c>
+      <c r="O165" s="4" t="inlineStr"/>
+      <c r="P165" s="4" t="inlineStr"/>
+      <c r="Q165" s="4" t="inlineStr"/>
+      <c r="R165" s="1" t="inlineStr"/>
+      <c r="S165" s="1" t="inlineStr"/>
+    </row>
+    <row r="166" customHeight="1" ht="3">
+      <c r="A166" s="1" t="inlineStr"/>
+      <c r="B166" s="1" t="inlineStr"/>
+      <c r="C166" s="1" t="inlineStr"/>
+      <c r="D166" s="1" t="inlineStr"/>
+      <c r="E166" s="1" t="inlineStr"/>
+      <c r="F166" s="1" t="inlineStr"/>
+      <c r="G166" s="1" t="inlineStr"/>
+      <c r="H166" s="1" t="inlineStr"/>
+      <c r="I166" s="1" t="inlineStr"/>
+      <c r="J166" s="1" t="inlineStr"/>
+      <c r="K166" s="1" t="inlineStr"/>
+      <c r="L166" s="1" t="inlineStr"/>
+      <c r="M166" s="1" t="inlineStr"/>
+      <c r="N166" s="1" t="inlineStr"/>
+      <c r="O166" s="1" t="inlineStr"/>
+      <c r="P166" s="1" t="inlineStr"/>
+      <c r="Q166" s="1" t="inlineStr"/>
+      <c r="R166" s="1" t="inlineStr"/>
+      <c r="S166" s="1" t="inlineStr"/>
+    </row>
+    <row r="167" customHeight="1" ht="20">
+      <c r="A167" s="1" t="inlineStr"/>
+      <c r="B167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">التاريخ</t>
+          </r>
+        </is>
+      </c>
+      <c r="C167" s="5" t="inlineStr"/>
+      <c r="D167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ملاحظات</t>
+          </r>
+        </is>
+      </c>
+      <c r="E167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">الوجهة</t>
+          </r>
+        </is>
+      </c>
+      <c r="F167" s="5" t="inlineStr"/>
+      <c r="G167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">المصفاة</t>
+          </r>
+        </is>
+      </c>
+      <c r="H167" s="5" t="inlineStr"/>
+      <c r="I167" s="5" t="inlineStr"/>
+      <c r="J167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">المادة</t>
+          </r>
+        </is>
+      </c>
+      <c r="K167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">الكمية</t>
+          </r>
+        </is>
+      </c>
+      <c r="L167" s="5" t="inlineStr"/>
+      <c r="M167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">السائق</t>
+          </r>
+        </is>
+      </c>
+      <c r="N167" s="5" t="inlineStr"/>
+      <c r="O167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">المعرف</t>
+          </r>
+        </is>
+      </c>
+      <c r="P167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">المركبة</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q167" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">No</t>
+          </r>
+        </is>
+      </c>
+      <c r="R167" s="5" t="inlineStr"/>
+      <c r="S167" s="1" t="inlineStr"/>
+    </row>
+    <row r="168" customHeight="1" ht="5">
+      <c r="A168" s="1" t="inlineStr"/>
+      <c r="B168" s="1" t="inlineStr"/>
+      <c r="C168" s="1" t="inlineStr"/>
+      <c r="D168" s="1" t="inlineStr"/>
+      <c r="E168" s="1" t="inlineStr"/>
+      <c r="F168" s="1" t="inlineStr"/>
+      <c r="G168" s="1" t="inlineStr"/>
+      <c r="H168" s="1" t="inlineStr"/>
+      <c r="I168" s="1" t="inlineStr"/>
+      <c r="J168" s="1" t="inlineStr"/>
+      <c r="K168" s="1" t="inlineStr"/>
+      <c r="L168" s="1" t="inlineStr"/>
+      <c r="M168" s="1" t="inlineStr"/>
+      <c r="N168" s="1" t="inlineStr"/>
+      <c r="O168" s="1" t="inlineStr"/>
+      <c r="P168" s="1" t="inlineStr"/>
+      <c r="Q168" s="1" t="inlineStr"/>
+      <c r="R168" s="1" t="inlineStr"/>
+      <c r="S168" s="1" t="inlineStr"/>
+    </row>
+    <row r="169" customHeight="1" ht="1">
+      <c r="A169" s="1" t="inlineStr"/>
+      <c r="B169" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-11T14:32:28</t>
+          </r>
+        </is>
+      </c>
+      <c r="C169" s="6" t="inlineStr"/>
+      <c r="D169" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">w</t>
+          </r>
+        </is>
+      </c>
+      <c r="E169" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F169" s="7" t="inlineStr"/>
+      <c r="G169" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H169" s="7" t="inlineStr"/>
+      <c r="I169" s="7" t="inlineStr"/>
+      <c r="J169" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K169" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">30000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L169" s="7" t="inlineStr"/>
+      <c r="M169" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">pers</t>
+          </r>
+        </is>
+      </c>
+      <c r="N169" s="7" t="inlineStr"/>
+      <c r="O169" s="1" t="inlineStr"/>
+      <c r="P169" s="1" t="inlineStr"/>
+      <c r="Q169" s="1" t="inlineStr"/>
+      <c r="R169" s="1" t="inlineStr"/>
+      <c r="S169" s="1" t="inlineStr"/>
+    </row>
+    <row r="170" customHeight="1" ht="29">
+      <c r="A170" s="1" t="inlineStr"/>
+      <c r="B170" s="6" t="inlineStr"/>
+      <c r="C170" s="6" t="inlineStr"/>
+      <c r="D170" s="7" t="inlineStr"/>
+      <c r="E170" s="7" t="inlineStr"/>
+      <c r="F170" s="7" t="inlineStr"/>
+      <c r="G170" s="7" t="inlineStr"/>
+      <c r="H170" s="7" t="inlineStr"/>
+      <c r="I170" s="7" t="inlineStr"/>
+      <c r="J170" s="7" t="inlineStr"/>
+      <c r="K170" s="7" t="inlineStr"/>
+      <c r="L170" s="7" t="inlineStr"/>
+      <c r="M170" s="7" t="inlineStr"/>
+      <c r="N170" s="7" t="inlineStr"/>
+      <c r="O170" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">71</t>
+          </r>
+        </is>
+      </c>
+      <c r="P170" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">980980</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q170" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">91</t>
+          </r>
+        </is>
+      </c>
+      <c r="R170" s="1" t="inlineStr"/>
+      <c r="S170" s="1" t="inlineStr"/>
+    </row>
+    <row r="171" customHeight="1" ht="1">
+      <c r="A171" s="1" t="inlineStr"/>
+      <c r="B171" s="1" t="inlineStr"/>
+      <c r="C171" s="1" t="inlineStr"/>
+      <c r="D171" s="1" t="inlineStr"/>
+      <c r="E171" s="1" t="inlineStr"/>
+      <c r="F171" s="1" t="inlineStr"/>
+      <c r="G171" s="1" t="inlineStr"/>
+      <c r="H171" s="1" t="inlineStr"/>
+      <c r="I171" s="1" t="inlineStr"/>
+      <c r="J171" s="1" t="inlineStr"/>
+      <c r="K171" s="1" t="inlineStr"/>
+      <c r="L171" s="1" t="inlineStr"/>
+      <c r="M171" s="1" t="inlineStr"/>
+      <c r="N171" s="1" t="inlineStr"/>
+      <c r="O171" s="7" t="inlineStr"/>
+      <c r="P171" s="7" t="inlineStr"/>
+      <c r="Q171" s="7" t="inlineStr"/>
+      <c r="R171" s="1" t="inlineStr"/>
+      <c r="S171" s="1" t="inlineStr"/>
+    </row>
+    <row r="172" customHeight="1" ht="5">
+      <c r="A172" s="1" t="inlineStr"/>
+      <c r="B172" s="1" t="inlineStr"/>
+      <c r="C172" s="1" t="inlineStr"/>
+      <c r="D172" s="1" t="inlineStr"/>
+      <c r="E172" s="1" t="inlineStr"/>
+      <c r="F172" s="1" t="inlineStr"/>
+      <c r="G172" s="1" t="inlineStr"/>
+      <c r="H172" s="1" t="inlineStr"/>
+      <c r="I172" s="1" t="inlineStr"/>
+      <c r="J172" s="1" t="inlineStr"/>
+      <c r="K172" s="1" t="inlineStr"/>
+      <c r="L172" s="1" t="inlineStr"/>
+      <c r="M172" s="1" t="inlineStr"/>
+      <c r="N172" s="1" t="inlineStr"/>
+      <c r="O172" s="1" t="inlineStr"/>
+      <c r="P172" s="1" t="inlineStr"/>
+      <c r="Q172" s="1" t="inlineStr"/>
+      <c r="R172" s="1" t="inlineStr"/>
+      <c r="S172" s="1" t="inlineStr"/>
+    </row>
+    <row r="173" customHeight="1" ht="1">
+      <c r="A173" s="1" t="inlineStr"/>
+      <c r="B173" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-11T15:44:23</t>
+          </r>
+        </is>
+      </c>
+      <c r="C173" s="6" t="inlineStr"/>
+      <c r="D173" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">w</t>
+          </r>
+        </is>
+      </c>
+      <c r="E173" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F173" s="7" t="inlineStr"/>
+      <c r="G173" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H173" s="7" t="inlineStr"/>
+      <c r="I173" s="7" t="inlineStr"/>
+      <c r="J173" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K173" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">6000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L173" s="7" t="inlineStr"/>
+      <c r="M173" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">pers</t>
+          </r>
+        </is>
+      </c>
+      <c r="N173" s="7" t="inlineStr"/>
+      <c r="O173" s="1" t="inlineStr"/>
+      <c r="P173" s="1" t="inlineStr"/>
+      <c r="Q173" s="1" t="inlineStr"/>
+      <c r="R173" s="1" t="inlineStr"/>
+      <c r="S173" s="1" t="inlineStr"/>
+    </row>
+    <row r="174" customHeight="1" ht="29">
+      <c r="A174" s="1" t="inlineStr"/>
+      <c r="B174" s="6" t="inlineStr"/>
+      <c r="C174" s="6" t="inlineStr"/>
+      <c r="D174" s="7" t="inlineStr"/>
+      <c r="E174" s="7" t="inlineStr"/>
+      <c r="F174" s="7" t="inlineStr"/>
+      <c r="G174" s="7" t="inlineStr"/>
+      <c r="H174" s="7" t="inlineStr"/>
+      <c r="I174" s="7" t="inlineStr"/>
+      <c r="J174" s="7" t="inlineStr"/>
+      <c r="K174" s="7" t="inlineStr"/>
+      <c r="L174" s="7" t="inlineStr"/>
+      <c r="M174" s="7" t="inlineStr"/>
+      <c r="N174" s="7" t="inlineStr"/>
+      <c r="O174" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">71</t>
+          </r>
+        </is>
+      </c>
+      <c r="P174" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">980980</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q174" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">96</t>
+          </r>
+        </is>
+      </c>
+      <c r="R174" s="1" t="inlineStr"/>
+      <c r="S174" s="1" t="inlineStr"/>
+    </row>
+    <row r="175" customHeight="1" ht="1">
+      <c r="A175" s="1" t="inlineStr"/>
+      <c r="B175" s="1" t="inlineStr"/>
+      <c r="C175" s="1" t="inlineStr"/>
+      <c r="D175" s="1" t="inlineStr"/>
+      <c r="E175" s="1" t="inlineStr"/>
+      <c r="F175" s="1" t="inlineStr"/>
+      <c r="G175" s="1" t="inlineStr"/>
+      <c r="H175" s="1" t="inlineStr"/>
+      <c r="I175" s="1" t="inlineStr"/>
+      <c r="J175" s="1" t="inlineStr"/>
+      <c r="K175" s="1" t="inlineStr"/>
+      <c r="L175" s="1" t="inlineStr"/>
+      <c r="M175" s="1" t="inlineStr"/>
+      <c r="N175" s="1" t="inlineStr"/>
+      <c r="O175" s="7" t="inlineStr"/>
+      <c r="P175" s="7" t="inlineStr"/>
+      <c r="Q175" s="7" t="inlineStr"/>
+      <c r="R175" s="1" t="inlineStr"/>
+      <c r="S175" s="1" t="inlineStr"/>
+    </row>
+    <row r="176" customHeight="1" ht="5">
+      <c r="A176" s="1" t="inlineStr"/>
+      <c r="B176" s="1" t="inlineStr"/>
+      <c r="C176" s="1" t="inlineStr"/>
+      <c r="D176" s="1" t="inlineStr"/>
+      <c r="E176" s="1" t="inlineStr"/>
+      <c r="F176" s="1" t="inlineStr"/>
+      <c r="G176" s="1" t="inlineStr"/>
+      <c r="H176" s="1" t="inlineStr"/>
+      <c r="I176" s="1" t="inlineStr"/>
+      <c r="J176" s="1" t="inlineStr"/>
+      <c r="K176" s="1" t="inlineStr"/>
+      <c r="L176" s="1" t="inlineStr"/>
+      <c r="M176" s="1" t="inlineStr"/>
+      <c r="N176" s="1" t="inlineStr"/>
+      <c r="O176" s="1" t="inlineStr"/>
+      <c r="P176" s="1" t="inlineStr"/>
+      <c r="Q176" s="1" t="inlineStr"/>
+      <c r="R176" s="1" t="inlineStr"/>
+      <c r="S176" s="1" t="inlineStr"/>
+    </row>
+    <row r="177" customHeight="1" ht="1">
+      <c r="A177" s="1" t="inlineStr"/>
+      <c r="B177" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-11T16:04:50</t>
+          </r>
+        </is>
+      </c>
+      <c r="C177" s="6" t="inlineStr"/>
+      <c r="D177" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">56</t>
+          </r>
+        </is>
+      </c>
+      <c r="E177" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F177" s="7" t="inlineStr"/>
+      <c r="G177" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H177" s="7" t="inlineStr"/>
+      <c r="I177" s="7" t="inlineStr"/>
+      <c r="J177" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K177" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">36000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L177" s="7" t="inlineStr"/>
+      <c r="M177" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">pers</t>
+          </r>
+        </is>
+      </c>
+      <c r="N177" s="7" t="inlineStr"/>
+      <c r="O177" s="1" t="inlineStr"/>
+      <c r="P177" s="1" t="inlineStr"/>
+      <c r="Q177" s="1" t="inlineStr"/>
+      <c r="R177" s="1" t="inlineStr"/>
+      <c r="S177" s="1" t="inlineStr"/>
+    </row>
+    <row r="178" customHeight="1" ht="29">
+      <c r="A178" s="1" t="inlineStr"/>
+      <c r="B178" s="6" t="inlineStr"/>
+      <c r="C178" s="6" t="inlineStr"/>
+      <c r="D178" s="7" t="inlineStr"/>
+      <c r="E178" s="7" t="inlineStr"/>
+      <c r="F178" s="7" t="inlineStr"/>
+      <c r="G178" s="7" t="inlineStr"/>
+      <c r="H178" s="7" t="inlineStr"/>
+      <c r="I178" s="7" t="inlineStr"/>
+      <c r="J178" s="7" t="inlineStr"/>
+      <c r="K178" s="7" t="inlineStr"/>
+      <c r="L178" s="7" t="inlineStr"/>
+      <c r="M178" s="7" t="inlineStr"/>
+      <c r="N178" s="7" t="inlineStr"/>
+      <c r="O178" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">72</t>
+          </r>
+        </is>
+      </c>
+      <c r="P178" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">980980</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q178" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">102</t>
+          </r>
+        </is>
+      </c>
+      <c r="R178" s="1" t="inlineStr"/>
+      <c r="S178" s="1" t="inlineStr"/>
+    </row>
+    <row r="179" customHeight="1" ht="1">
+      <c r="A179" s="1" t="inlineStr"/>
+      <c r="B179" s="1" t="inlineStr"/>
+      <c r="C179" s="1" t="inlineStr"/>
+      <c r="D179" s="1" t="inlineStr"/>
+      <c r="E179" s="1" t="inlineStr"/>
+      <c r="F179" s="1" t="inlineStr"/>
+      <c r="G179" s="1" t="inlineStr"/>
+      <c r="H179" s="1" t="inlineStr"/>
+      <c r="I179" s="1" t="inlineStr"/>
+      <c r="J179" s="1" t="inlineStr"/>
+      <c r="K179" s="1" t="inlineStr"/>
+      <c r="L179" s="1" t="inlineStr"/>
+      <c r="M179" s="1" t="inlineStr"/>
+      <c r="N179" s="1" t="inlineStr"/>
+      <c r="O179" s="7" t="inlineStr"/>
+      <c r="P179" s="7" t="inlineStr"/>
+      <c r="Q179" s="7" t="inlineStr"/>
+      <c r="R179" s="1" t="inlineStr"/>
+      <c r="S179" s="1" t="inlineStr"/>
+    </row>
+    <row r="180" customHeight="1" ht="5">
+      <c r="A180" s="1" t="inlineStr"/>
+      <c r="B180" s="1" t="inlineStr"/>
+      <c r="C180" s="1" t="inlineStr"/>
+      <c r="D180" s="1" t="inlineStr"/>
+      <c r="E180" s="1" t="inlineStr"/>
+      <c r="F180" s="1" t="inlineStr"/>
+      <c r="G180" s="1" t="inlineStr"/>
+      <c r="H180" s="1" t="inlineStr"/>
+      <c r="I180" s="1" t="inlineStr"/>
+      <c r="J180" s="1" t="inlineStr"/>
+      <c r="K180" s="1" t="inlineStr"/>
+      <c r="L180" s="1" t="inlineStr"/>
+      <c r="M180" s="1" t="inlineStr"/>
+      <c r="N180" s="1" t="inlineStr"/>
+      <c r="O180" s="1" t="inlineStr"/>
+      <c r="P180" s="1" t="inlineStr"/>
+      <c r="Q180" s="1" t="inlineStr"/>
+      <c r="R180" s="1" t="inlineStr"/>
+      <c r="S180" s="1" t="inlineStr"/>
+    </row>
+    <row r="181" customHeight="1" ht="1">
+      <c r="A181" s="1" t="inlineStr"/>
+      <c r="B181" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-13T14:49:18</t>
+          </r>
+        </is>
+      </c>
+      <c r="C181" s="6" t="inlineStr"/>
+      <c r="D181" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">trt</t>
+          </r>
+        </is>
+      </c>
+      <c r="E181" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F181" s="7" t="inlineStr"/>
+      <c r="G181" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H181" s="7" t="inlineStr"/>
+      <c r="I181" s="7" t="inlineStr"/>
+      <c r="J181" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K181" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">36000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L181" s="7" t="inlineStr"/>
+      <c r="M181" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">pers</t>
+          </r>
+        </is>
+      </c>
+      <c r="N181" s="7" t="inlineStr"/>
+      <c r="O181" s="1" t="inlineStr"/>
+      <c r="P181" s="1" t="inlineStr"/>
+      <c r="Q181" s="1" t="inlineStr"/>
+      <c r="R181" s="1" t="inlineStr"/>
+      <c r="S181" s="1" t="inlineStr"/>
+    </row>
+    <row r="182" customHeight="1" ht="29">
+      <c r="A182" s="1" t="inlineStr"/>
+      <c r="B182" s="6" t="inlineStr"/>
+      <c r="C182" s="6" t="inlineStr"/>
+      <c r="D182" s="7" t="inlineStr"/>
+      <c r="E182" s="7" t="inlineStr"/>
+      <c r="F182" s="7" t="inlineStr"/>
+      <c r="G182" s="7" t="inlineStr"/>
+      <c r="H182" s="7" t="inlineStr"/>
+      <c r="I182" s="7" t="inlineStr"/>
+      <c r="J182" s="7" t="inlineStr"/>
+      <c r="K182" s="7" t="inlineStr"/>
+      <c r="L182" s="7" t="inlineStr"/>
+      <c r="M182" s="7" t="inlineStr"/>
+      <c r="N182" s="7" t="inlineStr"/>
+      <c r="O182" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">70</t>
+          </r>
+        </is>
+      </c>
+      <c r="P182" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">980980</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q182" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">103</t>
+          </r>
+        </is>
+      </c>
+      <c r="R182" s="1" t="inlineStr"/>
+      <c r="S182" s="1" t="inlineStr"/>
+    </row>
+    <row r="183" customHeight="1" ht="1">
+      <c r="A183" s="1" t="inlineStr"/>
+      <c r="B183" s="1" t="inlineStr"/>
+      <c r="C183" s="1" t="inlineStr"/>
+      <c r="D183" s="1" t="inlineStr"/>
+      <c r="E183" s="1" t="inlineStr"/>
+      <c r="F183" s="1" t="inlineStr"/>
+      <c r="G183" s="1" t="inlineStr"/>
+      <c r="H183" s="1" t="inlineStr"/>
+      <c r="I183" s="1" t="inlineStr"/>
+      <c r="J183" s="1" t="inlineStr"/>
+      <c r="K183" s="1" t="inlineStr"/>
+      <c r="L183" s="1" t="inlineStr"/>
+      <c r="M183" s="1" t="inlineStr"/>
+      <c r="N183" s="1" t="inlineStr"/>
+      <c r="O183" s="7" t="inlineStr"/>
+      <c r="P183" s="7" t="inlineStr"/>
+      <c r="Q183" s="7" t="inlineStr"/>
+      <c r="R183" s="1" t="inlineStr"/>
+      <c r="S183" s="1" t="inlineStr"/>
+    </row>
+    <row r="184" customHeight="1" ht="5">
+      <c r="A184" s="1" t="inlineStr"/>
+      <c r="B184" s="1" t="inlineStr"/>
+      <c r="C184" s="1" t="inlineStr"/>
+      <c r="D184" s="1" t="inlineStr"/>
+      <c r="E184" s="1" t="inlineStr"/>
+      <c r="F184" s="1" t="inlineStr"/>
+      <c r="G184" s="1" t="inlineStr"/>
+      <c r="H184" s="1" t="inlineStr"/>
+      <c r="I184" s="1" t="inlineStr"/>
+      <c r="J184" s="1" t="inlineStr"/>
+      <c r="K184" s="1" t="inlineStr"/>
+      <c r="L184" s="1" t="inlineStr"/>
+      <c r="M184" s="1" t="inlineStr"/>
+      <c r="N184" s="1" t="inlineStr"/>
+      <c r="O184" s="1" t="inlineStr"/>
+      <c r="P184" s="1" t="inlineStr"/>
+      <c r="Q184" s="1" t="inlineStr"/>
+      <c r="R184" s="1" t="inlineStr"/>
+      <c r="S184" s="1" t="inlineStr"/>
+    </row>
+    <row r="185" customHeight="1" ht="1">
+      <c r="A185" s="1" t="inlineStr"/>
+      <c r="B185" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-13T14:51:15</t>
+          </r>
+        </is>
+      </c>
+      <c r="C185" s="6" t="inlineStr"/>
+      <c r="D185" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">tttt</t>
+          </r>
+        </is>
+      </c>
+      <c r="E185" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F185" s="7" t="inlineStr"/>
+      <c r="G185" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H185" s="7" t="inlineStr"/>
+      <c r="I185" s="7" t="inlineStr"/>
+      <c r="J185" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K185" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">45000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L185" s="7" t="inlineStr"/>
+      <c r="M185" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">another</t>
+          </r>
+        </is>
+      </c>
+      <c r="N185" s="7" t="inlineStr"/>
+      <c r="O185" s="1" t="inlineStr"/>
+      <c r="P185" s="1" t="inlineStr"/>
+      <c r="Q185" s="1" t="inlineStr"/>
+      <c r="R185" s="1" t="inlineStr"/>
+      <c r="S185" s="1" t="inlineStr"/>
+    </row>
+    <row r="186" customHeight="1" ht="29">
+      <c r="A186" s="1" t="inlineStr"/>
+      <c r="B186" s="6" t="inlineStr"/>
+      <c r="C186" s="6" t="inlineStr"/>
+      <c r="D186" s="7" t="inlineStr"/>
+      <c r="E186" s="7" t="inlineStr"/>
+      <c r="F186" s="7" t="inlineStr"/>
+      <c r="G186" s="7" t="inlineStr"/>
+      <c r="H186" s="7" t="inlineStr"/>
+      <c r="I186" s="7" t="inlineStr"/>
+      <c r="J186" s="7" t="inlineStr"/>
+      <c r="K186" s="7" t="inlineStr"/>
+      <c r="L186" s="7" t="inlineStr"/>
+      <c r="M186" s="7" t="inlineStr"/>
+      <c r="N186" s="7" t="inlineStr"/>
+      <c r="O186" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">68</t>
+          </r>
+        </is>
+      </c>
+      <c r="P186" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">321654</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q186" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">104</t>
+          </r>
+        </is>
+      </c>
+      <c r="R186" s="1" t="inlineStr"/>
+      <c r="S186" s="1" t="inlineStr"/>
+    </row>
+    <row r="187" customHeight="1" ht="1">
+      <c r="A187" s="1" t="inlineStr"/>
+      <c r="B187" s="1" t="inlineStr"/>
+      <c r="C187" s="1" t="inlineStr"/>
+      <c r="D187" s="1" t="inlineStr"/>
+      <c r="E187" s="1" t="inlineStr"/>
+      <c r="F187" s="1" t="inlineStr"/>
+      <c r="G187" s="1" t="inlineStr"/>
+      <c r="H187" s="1" t="inlineStr"/>
+      <c r="I187" s="1" t="inlineStr"/>
+      <c r="J187" s="1" t="inlineStr"/>
+      <c r="K187" s="1" t="inlineStr"/>
+      <c r="L187" s="1" t="inlineStr"/>
+      <c r="M187" s="1" t="inlineStr"/>
+      <c r="N187" s="1" t="inlineStr"/>
+      <c r="O187" s="7" t="inlineStr"/>
+      <c r="P187" s="7" t="inlineStr"/>
+      <c r="Q187" s="7" t="inlineStr"/>
+      <c r="R187" s="1" t="inlineStr"/>
+      <c r="S187" s="1" t="inlineStr"/>
+    </row>
+    <row r="188" customHeight="1" ht="5">
+      <c r="A188" s="1" t="inlineStr"/>
+      <c r="B188" s="1" t="inlineStr"/>
+      <c r="C188" s="1" t="inlineStr"/>
+      <c r="D188" s="1" t="inlineStr"/>
+      <c r="E188" s="1" t="inlineStr"/>
+      <c r="F188" s="1" t="inlineStr"/>
+      <c r="G188" s="1" t="inlineStr"/>
+      <c r="H188" s="1" t="inlineStr"/>
+      <c r="I188" s="1" t="inlineStr"/>
+      <c r="J188" s="1" t="inlineStr"/>
+      <c r="K188" s="1" t="inlineStr"/>
+      <c r="L188" s="1" t="inlineStr"/>
+      <c r="M188" s="1" t="inlineStr"/>
+      <c r="N188" s="1" t="inlineStr"/>
+      <c r="O188" s="1" t="inlineStr"/>
+      <c r="P188" s="1" t="inlineStr"/>
+      <c r="Q188" s="1" t="inlineStr"/>
+      <c r="R188" s="1" t="inlineStr"/>
+      <c r="S188" s="1" t="inlineStr"/>
+    </row>
+    <row r="189" customHeight="1" ht="1">
+      <c r="A189" s="1" t="inlineStr"/>
+      <c r="B189" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2023-11-13T20:01:16</t>
+          </r>
+        </is>
+      </c>
+      <c r="C189" s="6" t="inlineStr"/>
+      <c r="D189" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">gt</t>
+          </r>
+        </is>
+      </c>
+      <c r="E189" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">myTest</t>
+          </r>
+        </is>
+      </c>
+      <c r="F189" s="7" t="inlineStr"/>
+      <c r="G189" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ref1</t>
+          </r>
+        </is>
+      </c>
+      <c r="H189" s="7" t="inlineStr"/>
+      <c r="I189" s="7" t="inlineStr"/>
+      <c r="J189" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">mat2</t>
+          </r>
+        </is>
+      </c>
+      <c r="K189" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">45000</t>
+          </r>
+        </is>
+      </c>
+      <c r="L189" s="7" t="inlineStr"/>
+      <c r="M189" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">another</t>
+          </r>
+        </is>
+      </c>
+      <c r="N189" s="7" t="inlineStr"/>
+      <c r="O189" s="1" t="inlineStr"/>
+      <c r="P189" s="1" t="inlineStr"/>
+      <c r="Q189" s="1" t="inlineStr"/>
+      <c r="R189" s="1" t="inlineStr"/>
+      <c r="S189" s="1" t="inlineStr"/>
+    </row>
+    <row r="190" customHeight="1" ht="29">
+      <c r="A190" s="1" t="inlineStr"/>
+      <c r="B190" s="6" t="inlineStr"/>
+      <c r="C190" s="6" t="inlineStr"/>
+      <c r="D190" s="7" t="inlineStr"/>
+      <c r="E190" s="7" t="inlineStr"/>
+      <c r="F190" s="7" t="inlineStr"/>
+      <c r="G190" s="7" t="inlineStr"/>
+      <c r="H190" s="7" t="inlineStr"/>
+      <c r="I190" s="7" t="inlineStr"/>
+      <c r="J190" s="7" t="inlineStr"/>
+      <c r="K190" s="7" t="inlineStr"/>
+      <c r="L190" s="7" t="inlineStr"/>
+      <c r="M190" s="7" t="inlineStr"/>
+      <c r="N190" s="7" t="inlineStr"/>
+      <c r="O190" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">73</t>
+          </r>
+        </is>
+      </c>
+      <c r="P190" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">321654</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q190" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">105</t>
+          </r>
+        </is>
+      </c>
+      <c r="R190" s="1" t="inlineStr"/>
+      <c r="S190" s="1" t="inlineStr"/>
+    </row>
+    <row r="191" customHeight="1" ht="1">
+      <c r="A191" s="1" t="inlineStr"/>
+      <c r="B191" s="1" t="inlineStr"/>
+      <c r="C191" s="1" t="inlineStr"/>
+      <c r="D191" s="1" t="inlineStr"/>
+      <c r="E191" s="1" t="inlineStr"/>
+      <c r="F191" s="1" t="inlineStr"/>
+      <c r="G191" s="1" t="inlineStr"/>
+      <c r="H191" s="1" t="inlineStr"/>
+      <c r="I191" s="1" t="inlineStr"/>
+      <c r="J191" s="1" t="inlineStr"/>
+      <c r="K191" s="1" t="inlineStr"/>
+      <c r="L191" s="1" t="inlineStr"/>
+      <c r="M191" s="1" t="inlineStr"/>
+      <c r="N191" s="1" t="inlineStr"/>
+      <c r="O191" s="7" t="inlineStr"/>
+      <c r="P191" s="7" t="inlineStr"/>
+      <c r="Q191" s="7" t="inlineStr"/>
+      <c r="R191" s="1" t="inlineStr"/>
+      <c r="S191" s="1" t="inlineStr"/>
+    </row>
+    <row r="192" customHeight="1" ht="556">
+      <c r="A192" s="1" t="inlineStr"/>
+      <c r="B192" s="1" t="inlineStr"/>
+      <c r="C192" s="1" t="inlineStr"/>
+      <c r="D192" s="1" t="inlineStr"/>
+      <c r="E192" s="1" t="inlineStr"/>
+      <c r="F192" s="1" t="inlineStr"/>
+      <c r="G192" s="1" t="inlineStr"/>
+      <c r="H192" s="1" t="inlineStr"/>
+      <c r="I192" s="1" t="inlineStr"/>
+      <c r="J192" s="1" t="inlineStr"/>
+      <c r="K192" s="1" t="inlineStr"/>
+      <c r="L192" s="1" t="inlineStr"/>
+      <c r="M192" s="1" t="inlineStr"/>
+      <c r="N192" s="1" t="inlineStr"/>
+      <c r="O192" s="1" t="inlineStr"/>
+      <c r="P192" s="1" t="inlineStr"/>
+      <c r="Q192" s="1" t="inlineStr"/>
+      <c r="R192" s="1" t="inlineStr"/>
+      <c r="S192" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -6116,6 +7439,93 @@
     <mergeCell ref="O153:O154"/>
     <mergeCell ref="P153:P154"/>
     <mergeCell ref="Q153:Q154"/>
+    <mergeCell ref="B156:C157"/>
+    <mergeCell ref="D156:D157"/>
+    <mergeCell ref="E156:F157"/>
+    <mergeCell ref="G156:I157"/>
+    <mergeCell ref="J156:J157"/>
+    <mergeCell ref="K156:L157"/>
+    <mergeCell ref="M156:N157"/>
+    <mergeCell ref="O157:O158"/>
+    <mergeCell ref="P157:P158"/>
+    <mergeCell ref="Q157:Q158"/>
+    <mergeCell ref="B160:C161"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="E160:F161"/>
+    <mergeCell ref="G160:I161"/>
+    <mergeCell ref="J160:J161"/>
+    <mergeCell ref="K160:L161"/>
+    <mergeCell ref="M160:N161"/>
+    <mergeCell ref="O161:O162"/>
+    <mergeCell ref="P161:P162"/>
+    <mergeCell ref="Q161:Q162"/>
+    <mergeCell ref="N165:Q165"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="E167:F167"/>
+    <mergeCell ref="G167:I167"/>
+    <mergeCell ref="K167:L167"/>
+    <mergeCell ref="M167:N167"/>
+    <mergeCell ref="Q167:R167"/>
+    <mergeCell ref="B169:C170"/>
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="E169:F170"/>
+    <mergeCell ref="G169:I170"/>
+    <mergeCell ref="J169:J170"/>
+    <mergeCell ref="K169:L170"/>
+    <mergeCell ref="M169:N170"/>
+    <mergeCell ref="O170:O171"/>
+    <mergeCell ref="P170:P171"/>
+    <mergeCell ref="Q170:Q171"/>
+    <mergeCell ref="B173:C174"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="E173:F174"/>
+    <mergeCell ref="G173:I174"/>
+    <mergeCell ref="J173:J174"/>
+    <mergeCell ref="K173:L174"/>
+    <mergeCell ref="M173:N174"/>
+    <mergeCell ref="O174:O175"/>
+    <mergeCell ref="P174:P175"/>
+    <mergeCell ref="Q174:Q175"/>
+    <mergeCell ref="B177:C178"/>
+    <mergeCell ref="D177:D178"/>
+    <mergeCell ref="E177:F178"/>
+    <mergeCell ref="G177:I178"/>
+    <mergeCell ref="J177:J178"/>
+    <mergeCell ref="K177:L178"/>
+    <mergeCell ref="M177:N178"/>
+    <mergeCell ref="O178:O179"/>
+    <mergeCell ref="P178:P179"/>
+    <mergeCell ref="Q178:Q179"/>
+    <mergeCell ref="B181:C182"/>
+    <mergeCell ref="D181:D182"/>
+    <mergeCell ref="E181:F182"/>
+    <mergeCell ref="G181:I182"/>
+    <mergeCell ref="J181:J182"/>
+    <mergeCell ref="K181:L182"/>
+    <mergeCell ref="M181:N182"/>
+    <mergeCell ref="O182:O183"/>
+    <mergeCell ref="P182:P183"/>
+    <mergeCell ref="Q182:Q183"/>
+    <mergeCell ref="B185:C186"/>
+    <mergeCell ref="D185:D186"/>
+    <mergeCell ref="E185:F186"/>
+    <mergeCell ref="G185:I186"/>
+    <mergeCell ref="J185:J186"/>
+    <mergeCell ref="K185:L186"/>
+    <mergeCell ref="M185:N186"/>
+    <mergeCell ref="O186:O187"/>
+    <mergeCell ref="P186:P187"/>
+    <mergeCell ref="Q186:Q187"/>
+    <mergeCell ref="B189:C190"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="E189:F190"/>
+    <mergeCell ref="G189:I190"/>
+    <mergeCell ref="J189:J190"/>
+    <mergeCell ref="K189:L190"/>
+    <mergeCell ref="M189:N190"/>
+    <mergeCell ref="O190:O191"/>
+    <mergeCell ref="P190:P191"/>
+    <mergeCell ref="Q190:Q191"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.00" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>